<commit_message>
Starting on DTU in earnest
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
+++ b/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10032" windowHeight="7020" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10035" windowHeight="7020"/>
   </bookViews>
   <sheets>
     <sheet name="foes" sheetId="5" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1016" uniqueCount="403">
   <si>
     <t>name</t>
   </si>
@@ -623,276 +623,90 @@
     <t>{yieldsSymbol}8{wildAttack}8{repairSymbol}</t>
   </si>
   <si>
-    <t>06.1.0-AnimalcularCloud</t>
-  </si>
-  <si>
     <t>foe</t>
   </si>
   <si>
-    <t>AnimalcularCloud</t>
-  </si>
-  <si>
     <t>{fireSymbol}</t>
   </si>
   <si>
-    <t>{damageSymbol}</t>
-  </si>
-  <si>
-    <t>06.1.1-Drone</t>
-  </si>
-  <si>
     <t>Drone</t>
   </si>
   <si>
     <t>{bulletsSymbol}</t>
   </si>
   <si>
-    <t>06.1.2-Killbot</t>
-  </si>
-  <si>
     <t>Killbot</t>
   </si>
   <si>
     <t>{electricitySymbol}</t>
   </si>
   <si>
-    <t>06.1.3-Mycohemoth</t>
-  </si>
-  <si>
     <t>Mycohemoth</t>
   </si>
   <si>
     <t>{punchSymbol}</t>
   </si>
   <si>
-    <t>06.1.4-Cloudshark</t>
-  </si>
-  <si>
     <t>Cloudshark</t>
   </si>
   <si>
     <t>{scratchSymbol}</t>
   </si>
   <si>
-    <t>06.1.5-Leviathan</t>
-  </si>
-  <si>
     <t>Leviathan</t>
   </si>
   <si>
     <t>{acidSymbol}</t>
   </si>
   <si>
-    <t>06.2.0-Puffer</t>
-  </si>
-  <si>
     <t>Puffer</t>
   </si>
   <si>
-    <t>06.2.1-Kumonga</t>
-  </si>
-  <si>
-    <t>Kumonga</t>
-  </si>
-  <si>
-    <t>06.2.2-LandKraken</t>
-  </si>
-  <si>
     <t>Land Kraken</t>
   </si>
   <si>
-    <t>06.2.3-Megaspawn</t>
-  </si>
-  <si>
-    <t>Megaspawn</t>
-  </si>
-  <si>
-    <t>06.2.4-Scout</t>
-  </si>
-  <si>
     <t>Scout</t>
   </si>
   <si>
-    <t>06.2.5-AureliaOptirapax</t>
-  </si>
-  <si>
     <t>Aurelia Optirapax</t>
   </si>
   <si>
-    <t>06.2.6-Probe</t>
-  </si>
-  <si>
-    <t>Probe</t>
-  </si>
-  <si>
-    <t>06.2.7-TerrorShip</t>
-  </si>
-  <si>
-    <t>Terror Ship</t>
-  </si>
-  <si>
-    <t>06.3.0-PlagueBot</t>
-  </si>
-  <si>
     <t>PlagueBot</t>
   </si>
   <si>
-    <t>06.3.1-Shambler</t>
-  </si>
-  <si>
     <t>Shambler</t>
   </si>
   <si>
-    <t>06.3.2-AttackShip</t>
-  </si>
-  <si>
-    <t>Attack Ship</t>
-  </si>
-  <si>
-    <t>06.3.3-Ultralisk</t>
-  </si>
-  <si>
-    <t>Ultralisk</t>
-  </si>
-  <si>
-    <t>06.3.4-Megaguirus</t>
-  </si>
-  <si>
-    <t>Megaguirus</t>
-  </si>
-  <si>
-    <t>06.3.5-Berserker</t>
-  </si>
-  <si>
     <t>Berserker</t>
   </si>
   <si>
-    <t>06.3.6-Lurker</t>
-  </si>
-  <si>
     <t>Lurker</t>
   </si>
   <si>
-    <t>06.3.7-BirgusGiganticus</t>
-  </si>
-  <si>
-    <t>Birgus Giganticus</t>
-  </si>
-  <si>
-    <t>06.3.8-Akkorokaumi</t>
-  </si>
-  <si>
-    <t>Akkorokaumi</t>
-  </si>
-  <si>
-    <t>06.3.9-MechaDragon</t>
-  </si>
-  <si>
     <t>MechaDragon</t>
   </si>
   <si>
-    <t>06.3.10-Hedora</t>
-  </si>
-  <si>
-    <t>Hedora</t>
-  </si>
-  <si>
-    <t>06.3.11-Abductor</t>
-  </si>
-  <si>
     <t>Abductor</t>
   </si>
   <si>
-    <t>06.4.0-Daidarabochi</t>
-  </si>
-  <si>
-    <t>Daidarabochi</t>
-  </si>
-  <si>
-    <t>06.4.1-Destroyer</t>
-  </si>
-  <si>
     <t>Destroyer</t>
   </si>
   <si>
-    <t>06.4.2-Orga</t>
-  </si>
-  <si>
-    <t>Orga</t>
-  </si>
-  <si>
-    <t>06.4.3-Hydra</t>
-  </si>
-  <si>
     <t>Hydra</t>
   </si>
   <si>
-    <t>06.4.4-Typhon</t>
-  </si>
-  <si>
     <t>Typhon</t>
   </si>
   <si>
-    <t>06.4.5-Bomber</t>
-  </si>
-  <si>
-    <t>Bomber</t>
-  </si>
-  <si>
-    <t>06.4.6-Defiler</t>
-  </si>
-  <si>
-    <t>Defiler</t>
-  </si>
-  <si>
-    <t>06.4.7-Guard</t>
-  </si>
-  <si>
     <t>Guard</t>
   </si>
   <si>
-    <t>06.5.0-Battleship</t>
-  </si>
-  <si>
-    <t>Battleship</t>
-  </si>
-  <si>
-    <t>06.5.1-Rakshasa</t>
-  </si>
-  <si>
     <t>Rakshasa</t>
   </si>
   <si>
-    <t>06.5.2-Canid</t>
-  </si>
-  <si>
-    <t>Canid</t>
-  </si>
-  <si>
-    <t>06.5.3-Biollante</t>
-  </si>
-  <si>
-    <t>Biollante</t>
-  </si>
-  <si>
-    <t>06.5.4-Ghidoran</t>
-  </si>
-  <si>
-    <t>Ghidoran</t>
-  </si>
-  <si>
-    <t>06.5.5-Jormungand</t>
-  </si>
-  <si>
     <t>Jormungand</t>
   </si>
   <si>
-    <t>06.6.0-Mothership</t>
-  </si>
-  <si>
-    <t>{foeCard}</t>
-  </si>
-  <si>
     <t>06.7.1-BrainSucker</t>
   </si>
   <si>
@@ -1088,9 +902,6 @@
     <t>{fireSymbol}{bulletsSymbol}</t>
   </si>
   <si>
-    <t>{damageSymbol}{damageSymbol}</t>
-  </si>
-  <si>
     <t>{fireSymbol}{punchSymbol}</t>
   </si>
   <si>
@@ -1112,18 +923,6 @@
     <t>{scratchSymbol}{acidSymbol}</t>
   </si>
   <si>
-    <t>{damageSymbol}{damageSymbol}\n{damageSymbol}{damageSymbol}</t>
-  </si>
-  <si>
-    <t>{damageSymbol}{damageSymbol}\n{damageSymbol}{damageSymbol}{damageSymbol}</t>
-  </si>
-  <si>
-    <t>{damageSymbol}{damageSymbol}{damageSymbol}\n{damageSymbol}{damageSymbol}{damageSymbol}</t>
-  </si>
-  <si>
-    <t>{damageSymbol}\n{damageSymbol}{damageSymbol}</t>
-  </si>
-  <si>
     <t>{fireSymbol}\n{bulletsSymbol}{electricitySymbol}</t>
   </si>
   <si>
@@ -1205,28 +1004,235 @@
     <t>{bulletsSymbol}{electricitySymbol}\n{punchSymbol}{scratchSymbol}{acidSymbol}</t>
   </si>
   <si>
-    <t>Players may not trade cards.</t>
-  </si>
-  <si>
-    <t>Moves to the nearest city when moving.</t>
-  </si>
-  <si>
-    <t>Look at -1 card when drawing.</t>
-  </si>
-  <si>
-    <t>Discard 3 scientists.</t>
-  </si>
-  <si>
-    <t>Add a new alien in transit.</t>
-  </si>
-  <si>
-    <t>4 Escorts,\nMoves to largest pile.</t>
-  </si>
-  <si>
     <t>SampleMonster.png</t>
   </si>
   <si>
-    <t>Mothership</t>
+    <t>06.1.1</t>
+  </si>
+  <si>
+    <t>06.1.2</t>
+  </si>
+  <si>
+    <t>06.1.3</t>
+  </si>
+  <si>
+    <t>06.1.4</t>
+  </si>
+  <si>
+    <t>06.1.5</t>
+  </si>
+  <si>
+    <t>06.1.6</t>
+  </si>
+  <si>
+    <t>06.2.1</t>
+  </si>
+  <si>
+    <t>06.2.2</t>
+  </si>
+  <si>
+    <t>06.2.3</t>
+  </si>
+  <si>
+    <t>06.2.4</t>
+  </si>
+  <si>
+    <t>06.2.5</t>
+  </si>
+  <si>
+    <t>06.2.6</t>
+  </si>
+  <si>
+    <t>06.2.7</t>
+  </si>
+  <si>
+    <t>06.2.8</t>
+  </si>
+  <si>
+    <t>06.3.1</t>
+  </si>
+  <si>
+    <t>06.3.2</t>
+  </si>
+  <si>
+    <t>06.3.3</t>
+  </si>
+  <si>
+    <t>06.3.4</t>
+  </si>
+  <si>
+    <t>06.3.5</t>
+  </si>
+  <si>
+    <t>06.3.6</t>
+  </si>
+  <si>
+    <t>06.3.7</t>
+  </si>
+  <si>
+    <t>06.3.8</t>
+  </si>
+  <si>
+    <t>06.3.9</t>
+  </si>
+  <si>
+    <t>06.3.10</t>
+  </si>
+  <si>
+    <t>06.3.11</t>
+  </si>
+  <si>
+    <t>06.3.12</t>
+  </si>
+  <si>
+    <t>06.4.1</t>
+  </si>
+  <si>
+    <t>06.4.2</t>
+  </si>
+  <si>
+    <t>06.4.3</t>
+  </si>
+  <si>
+    <t>06.4.4</t>
+  </si>
+  <si>
+    <t>06.4.5</t>
+  </si>
+  <si>
+    <t>06.4.6</t>
+  </si>
+  <si>
+    <t>06.4.7</t>
+  </si>
+  <si>
+    <t>06.4.8</t>
+  </si>
+  <si>
+    <t>06.5.1</t>
+  </si>
+  <si>
+    <t>06.5.2</t>
+  </si>
+  <si>
+    <t>06.5.3</t>
+  </si>
+  <si>
+    <t>06.5.4</t>
+  </si>
+  <si>
+    <t>06.5.5</t>
+  </si>
+  <si>
+    <t>06.5.6</t>
+  </si>
+  <si>
+    <t>06.6.1</t>
+  </si>
+  <si>
+    <t>1{damageSymbol}</t>
+  </si>
+  <si>
+    <t>2{damageSymbol}</t>
+  </si>
+  <si>
+    <t>3{damageSymbol}</t>
+  </si>
+  <si>
+    <t>4{damageSymbol}</t>
+  </si>
+  <si>
+    <t>5{damageSymbol}</t>
+  </si>
+  <si>
+    <t>6{damageSymbol}</t>
+  </si>
+  <si>
+    <t>Animalcular Cloud</t>
+  </si>
+  <si>
+    <t>Fury Beast</t>
+  </si>
+  <si>
+    <t>Terror Beast</t>
+  </si>
+  <si>
+    <t>Blaster</t>
+  </si>
+  <si>
+    <t>Berthaly</t>
+  </si>
+  <si>
+    <t>Spionga</t>
+  </si>
+  <si>
+    <t>Megasaur</t>
+  </si>
+  <si>
+    <t>Gigantanulon</t>
+  </si>
+  <si>
+    <t>Birgus Gigantus</t>
+  </si>
+  <si>
+    <t>Akkorokamui</t>
+  </si>
+  <si>
+    <t>Kaidoro</t>
+  </si>
+  <si>
+    <t>Daidarabotchi</t>
+  </si>
+  <si>
+    <t>Milorg</t>
+  </si>
+  <si>
+    <t>Walking Bomb</t>
+  </si>
+  <si>
+    <t>King Kaiju</t>
+  </si>
+  <si>
+    <t>Gargantulus</t>
+  </si>
+  <si>
+    <t>06.7.1</t>
+  </si>
+  <si>
+    <t>7{damageSymbol}</t>
+  </si>
+  <si>
+    <t>Lich Queen</t>
+  </si>
+  <si>
+    <t>Borovi</t>
+  </si>
+  <si>
+    <t>Matsil</t>
+  </si>
+  <si>
+    <t>Rokap</t>
+  </si>
+  <si>
+    <t>Vorsa</t>
+  </si>
+  <si>
+    <t>{beast}</t>
+  </si>
+  <si>
+    <t>{flier}</t>
+  </si>
+  <si>
+    <t>{robot}</t>
+  </si>
+  <si>
+    <t>{plant}</t>
+  </si>
+  <si>
+    <t>{undead}</t>
+  </si>
+  <si>
+    <t>{abomination}</t>
   </si>
 </sst>
 </file>
@@ -1300,7 +1306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1308,6 +1314,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2320,26 +2327,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I42"/>
+  <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="91.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="47.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="98.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="91.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="47.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2365,1126 +2372,1141 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>200</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>203</v>
+        <v>368</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>204</v>
+        <v>328</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>53</v>
+        <v>398</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="I3" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>207</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E4" s="2" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>203</v>
+        <v>368</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>210</v>
+        <v>330</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>115</v>
+        <v>400</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>211</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="I5" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>213</v>
+        <v>331</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>49</v>
+        <v>401</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>214</v>
+        <v>201</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>203</v>
+        <v>368</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>216</v>
+        <v>332</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>402</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>203</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>368</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>219</v>
+        <v>333</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>115</v>
+        <v>397</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>220</v>
+        <v>375</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>353</v>
+        <v>291</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>334</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>398</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>222</v>
+        <v>374</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>355</v>
+        <v>292</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I9" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>224</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>356</v>
+        <v>293</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>225</v>
+        <v>336</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>400</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>226</v>
+        <v>205</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>357</v>
+        <v>294</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>227</v>
+        <v>337</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>53</v>
+        <v>401</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>228</v>
+        <v>379</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>358</v>
+        <v>295</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>229</v>
+        <v>338</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>39</v>
+        <v>402</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>230</v>
+        <v>380</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>359</v>
+        <v>296</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+        <v>369</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>231</v>
+        <v>339</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>53</v>
+        <v>397</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>232</v>
+        <v>376</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>360</v>
+        <v>297</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>354</v>
+        <v>369</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>233</v>
+        <v>340</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>53</v>
+        <v>398</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>234</v>
+        <v>214</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>361</v>
+        <v>298</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="I15" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>35</v>
-      </c>
       <c r="E16" s="2" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>366</v>
+        <v>299</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>237</v>
+        <v>342</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>39</v>
+        <v>400</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>238</v>
+        <v>377</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>367</v>
+        <v>300</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>239</v>
+        <v>343</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>401</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>240</v>
+        <v>216</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>368</v>
+        <v>301</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>241</v>
+        <v>344</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>44</v>
+        <v>402</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>242</v>
+        <v>381</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>369</v>
+        <v>302</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I19" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>243</v>
+        <v>345</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>49</v>
+        <v>397</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>244</v>
+        <v>378</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>370</v>
+        <v>303</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>245</v>
+        <v>346</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>35</v>
+        <v>398</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>246</v>
+        <v>218</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>371</v>
+        <v>304</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I21" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>347</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
-        <v>247</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="E22" s="2" t="s">
-        <v>248</v>
+        <v>215</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>372</v>
+        <v>305</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>249</v>
+        <v>348</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>44</v>
+        <v>400</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>250</v>
+        <v>383</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>373</v>
+        <v>306</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>251</v>
+        <v>349</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>44</v>
+        <v>401</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>252</v>
+        <v>382</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>374</v>
+        <v>307</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>253</v>
+        <v>350</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>35</v>
+        <v>402</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>254</v>
+        <v>384</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>375</v>
+        <v>308</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+        <v>370</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>255</v>
+        <v>351</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>44</v>
+        <v>397</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>376</v>
+        <v>309</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>257</v>
+        <v>352</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>53</v>
+        <v>398</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>258</v>
+        <v>219</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>377</v>
+        <v>310</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>365</v>
-      </c>
-      <c r="I27" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>353</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
-        <v>259</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>260</v>
+        <v>217</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>378</v>
+        <v>311</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>261</v>
+        <v>354</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>53</v>
+        <v>400</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>262</v>
+        <v>386</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>379</v>
+        <v>312</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>263</v>
+        <v>355</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>49</v>
+        <v>401</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>264</v>
+        <v>385</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>380</v>
+        <v>313</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>265</v>
+        <v>356</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>44</v>
+        <v>402</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>266</v>
+        <v>387</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>381</v>
+        <v>314</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>267</v>
+        <v>357</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>44</v>
+        <v>397</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>268</v>
+        <v>222</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>382</v>
+        <v>315</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>269</v>
+        <v>358</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>53</v>
+        <v>398</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>270</v>
+        <v>223</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>383</v>
+        <v>316</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="I33" s="2" t="s">
+        <v>371</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="s">
-        <v>271</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C34" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D34" s="2" t="s">
-        <v>39</v>
-      </c>
       <c r="E34" s="2" t="s">
-        <v>272</v>
+        <v>221</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>384</v>
+        <v>317</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>273</v>
+        <v>360</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>53</v>
+        <v>400</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>274</v>
+        <v>396</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>385</v>
+        <v>318</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
-        <v>362</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+        <v>371</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>275</v>
+        <v>361</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>53</v>
+        <v>401</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>276</v>
+        <v>226</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>387</v>
+        <v>320</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="F37" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G37" s="3"/>
+      <c r="H37" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>363</v>
       </c>
-      <c r="I36" s="2" t="s">
+      <c r="B38" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="F39" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="G39" s="3"/>
+      <c r="H39" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A37" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="B37" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="F37" s="3" t="s">
+      <c r="E40" s="2" t="s">
+        <v>389</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="F41" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="G42" s="2"/>
+      <c r="H42" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="7" t="s">
+        <v>390</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C43" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>402</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>388</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>393</v>
-      </c>
-      <c r="H37" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="B38" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D38" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E38" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="F38" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="G38" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A39" s="3" t="s">
-        <v>281</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="F39" s="3" t="s">
-        <v>390</v>
-      </c>
-      <c r="G39" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="H39" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="s">
-        <v>283</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="F40" s="2" t="s">
+      <c r="F43" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="G40" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A41" s="3" t="s">
-        <v>285</v>
-      </c>
-      <c r="B41" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C41" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>286</v>
-      </c>
-      <c r="F41" s="3" t="s">
-        <v>392</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>363</v>
-      </c>
-      <c r="I41" s="2" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>288</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="F42" s="2" t="s">
-        <v>386</v>
-      </c>
-      <c r="G42" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="I42" s="2" t="s">
-        <v>399</v>
+      <c r="I43" s="7" t="s">
+        <v>326</v>
       </c>
     </row>
   </sheetData>
@@ -3497,25 +3519,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="56.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="4.44140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="56.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3544,19 +3566,19 @@
         <v>14</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>334</v>
+        <v>272</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>336</v>
+        <v>274</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>337</v>
+        <v>275</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -3573,7 +3595,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>339</v>
+        <v>277</v>
       </c>
       <c r="G2" s="5"/>
       <c r="H2" s="5"/>
@@ -3581,7 +3603,7 @@
         <v>20</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K2" t="str">
         <f t="shared" ref="K2:K18" si="0">IF(ISBLANK(G2), "", "{cc}")</f>
@@ -3596,7 +3618,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>21</v>
       </c>
@@ -3613,7 +3635,7 @@
         <v>22</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>340</v>
+        <v>278</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="5"/>
@@ -3621,7 +3643,7 @@
         <v>20</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K3" t="str">
         <f t="shared" si="0"/>
@@ -3636,7 +3658,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>23</v>
       </c>
@@ -3653,7 +3675,7 @@
         <v>24</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>341</v>
+        <v>279</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
@@ -3661,7 +3683,7 @@
         <v>20</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K4" t="str">
         <f t="shared" si="0"/>
@@ -3676,7 +3698,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>25</v>
       </c>
@@ -3693,7 +3715,7 @@
         <v>26</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>342</v>
+        <v>280</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="5"/>
@@ -3701,7 +3723,7 @@
         <v>27</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K5" t="str">
         <f t="shared" si="0"/>
@@ -3716,7 +3738,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>28</v>
       </c>
@@ -3733,7 +3755,7 @@
         <v>29</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>343</v>
+        <v>281</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="5"/>
@@ -3741,7 +3763,7 @@
         <v>30</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K6" t="str">
         <f t="shared" si="0"/>
@@ -3756,7 +3778,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>31</v>
       </c>
@@ -3773,7 +3795,7 @@
         <v>32</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>344</v>
+        <v>282</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
@@ -3781,7 +3803,7 @@
         <v>30</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K7" t="str">
         <f t="shared" si="0"/>
@@ -3796,7 +3818,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>68</v>
       </c>
@@ -3821,7 +3843,7 @@
         <v>20</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K8" t="str">
         <f t="shared" si="0"/>
@@ -3836,7 +3858,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>72</v>
       </c>
@@ -3861,7 +3883,7 @@
         <v>27</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K9" t="str">
         <f t="shared" si="0"/>
@@ -3876,7 +3898,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>75</v>
       </c>
@@ -3901,7 +3923,7 @@
         <v>56</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K10" t="str">
         <f t="shared" si="0"/>
@@ -3916,7 +3938,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>78</v>
       </c>
@@ -3941,7 +3963,7 @@
         <v>47</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K11" t="str">
         <f t="shared" si="0"/>
@@ -3956,7 +3978,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>81</v>
       </c>
@@ -3973,7 +3995,7 @@
         <v>82</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>345</v>
+        <v>283</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="5"/>
@@ -3981,7 +4003,7 @@
         <v>47</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K12" t="str">
         <f t="shared" si="0"/>
@@ -3996,7 +4018,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>94</v>
       </c>
@@ -4021,7 +4043,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K13" t="str">
         <f t="shared" si="0"/>
@@ -4036,7 +4058,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>98</v>
       </c>
@@ -4053,7 +4075,7 @@
         <v>99</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>346</v>
+        <v>284</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
@@ -4061,7 +4083,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K14" t="str">
         <f t="shared" si="0"/>
@@ -4076,7 +4098,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>100</v>
       </c>
@@ -4093,7 +4115,7 @@
         <v>101</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>347</v>
+        <v>285</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="5"/>
@@ -4101,7 +4123,7 @@
         <v>30</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K15" t="str">
         <f t="shared" si="0"/>
@@ -4116,7 +4138,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>102</v>
       </c>
@@ -4133,7 +4155,7 @@
         <v>103</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>348</v>
+        <v>286</v>
       </c>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
@@ -4141,7 +4163,7 @@
         <v>20</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K16" t="str">
         <f t="shared" si="0"/>
@@ -4156,7 +4178,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>104</v>
       </c>
@@ -4181,7 +4203,7 @@
         <v>30</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K17" t="str">
         <f t="shared" si="0"/>
@@ -4196,7 +4218,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>106</v>
       </c>
@@ -4213,7 +4235,7 @@
         <v>107</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>349</v>
+        <v>287</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>20</v>
@@ -4223,7 +4245,7 @@
         <v>20</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="K18" t="str">
         <f t="shared" si="0"/>
@@ -4252,25 +4274,25 @@
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4302,19 +4324,19 @@
         <v>13</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>334</v>
+        <v>272</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>335</v>
+        <v>273</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>336</v>
+        <v>274</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -4331,7 +4353,7 @@
         <v>132</v>
       </c>
       <c r="G2" t="s">
-        <v>350</v>
+        <v>288</v>
       </c>
       <c r="H2" t="s">
         <v>133</v>
@@ -4343,7 +4365,7 @@
         <v>56</v>
       </c>
       <c r="K2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L2" t="str">
         <f t="shared" ref="L2:N7" si="0">IF(ISBLANK(H2), "", "{cc}")</f>
@@ -4358,7 +4380,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>134</v>
       </c>
@@ -4384,7 +4406,7 @@
         <v>56</v>
       </c>
       <c r="K3" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L3" t="str">
         <f t="shared" si="0"/>
@@ -4399,7 +4421,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>137</v>
       </c>
@@ -4428,7 +4450,7 @@
         <v>56</v>
       </c>
       <c r="K4" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L4" t="str">
         <f t="shared" si="0"/>
@@ -4443,7 +4465,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>140</v>
       </c>
@@ -4469,7 +4491,7 @@
         <v>142</v>
       </c>
       <c r="K5" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L5" t="str">
         <f t="shared" si="0"/>
@@ -4484,7 +4506,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>143</v>
       </c>
@@ -4513,7 +4535,7 @@
         <v>56</v>
       </c>
       <c r="K6" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L6" t="str">
         <f t="shared" si="0"/>
@@ -4528,7 +4550,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>146</v>
       </c>
@@ -4545,7 +4567,7 @@
         <v>147</v>
       </c>
       <c r="G7" t="s">
-        <v>351</v>
+        <v>289</v>
       </c>
       <c r="H7" t="s">
         <v>139</v>
@@ -4557,7 +4579,7 @@
         <v>42</v>
       </c>
       <c r="K7" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L7" t="str">
         <f t="shared" si="0"/>
@@ -4572,7 +4594,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>148</v>
       </c>
@@ -4604,7 +4626,7 @@
         <v>42</v>
       </c>
       <c r="K8" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L8" t="str">
         <f t="shared" ref="L8:L12" si="1">IF(ISBLANK(H8), "", "{cc}")</f>
@@ -4619,7 +4641,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>150</v>
       </c>
@@ -4651,7 +4673,7 @@
         <v>42</v>
       </c>
       <c r="K9" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L9" t="str">
         <f t="shared" si="1"/>
@@ -4666,7 +4688,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>152</v>
       </c>
@@ -4695,7 +4717,7 @@
         <v>133</v>
       </c>
       <c r="K10" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L10" t="str">
         <f t="shared" si="1"/>
@@ -4710,7 +4732,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>155</v>
       </c>
@@ -4742,7 +4764,7 @@
         <v>142</v>
       </c>
       <c r="K11" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L11" t="str">
         <f t="shared" si="1"/>
@@ -4757,7 +4779,7 @@
         <v>{cc}</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>158</v>
       </c>
@@ -4786,7 +4808,7 @@
         <v>142</v>
       </c>
       <c r="K12" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
       <c r="L12" t="str">
         <f t="shared" si="1"/>
@@ -4818,23 +4840,23 @@
       <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="86.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="10" max="10" width="10.44140625" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" customWidth="1"/>
-    <col min="12" max="12" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="86.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" customWidth="1"/>
+    <col min="12" max="12" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -4869,10 +4891,10 @@
         <v>14</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>33</v>
       </c>
@@ -4901,10 +4923,10 @@
         <v>30</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>38</v>
       </c>
@@ -4933,10 +4955,10 @@
         <v>42</v>
       </c>
       <c r="L3" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>43</v>
       </c>
@@ -4965,10 +4987,10 @@
         <v>47</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>48</v>
       </c>
@@ -4997,10 +5019,10 @@
         <v>27</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>52</v>
       </c>
@@ -5029,10 +5051,10 @@
         <v>56</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>57</v>
       </c>
@@ -5061,10 +5083,10 @@
         <v>56</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>60</v>
       </c>
@@ -5093,10 +5115,10 @@
         <v>64</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>65</v>
       </c>
@@ -5125,10 +5147,10 @@
         <v>27</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>83</v>
       </c>
@@ -5157,10 +5179,10 @@
         <v>20</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>85</v>
       </c>
@@ -5189,10 +5211,10 @@
         <v>30</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>87</v>
       </c>
@@ -5221,10 +5243,10 @@
         <v>27</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>89</v>
       </c>
@@ -5253,10 +5275,10 @@
         <v>56</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>92</v>
       </c>
@@ -5285,10 +5307,10 @@
         <v>64</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>109</v>
       </c>
@@ -5317,10 +5339,10 @@
         <v>64</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>111</v>
       </c>
@@ -5349,10 +5371,10 @@
         <v>27</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>114</v>
       </c>
@@ -5379,10 +5401,10 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>117</v>
       </c>
@@ -5411,10 +5433,10 @@
         <v>20</v>
       </c>
       <c r="L18" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>120</v>
       </c>
@@ -5443,10 +5465,10 @@
         <v>20</v>
       </c>
       <c r="L19" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>122</v>
       </c>
@@ -5475,10 +5497,10 @@
         <v>20</v>
       </c>
       <c r="L20" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>125</v>
       </c>
@@ -5509,10 +5531,10 @@
         <v>20</v>
       </c>
       <c r="L21" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>127</v>
       </c>
@@ -5543,10 +5565,10 @@
         <v>64</v>
       </c>
       <c r="L22" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>160</v>
       </c>
@@ -5573,10 +5595,10 @@
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
       <c r="L23" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>164</v>
       </c>
@@ -5603,10 +5625,10 @@
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
       <c r="L24" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>167</v>
       </c>
@@ -5633,10 +5655,10 @@
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
       <c r="L25" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>170</v>
       </c>
@@ -5663,10 +5685,10 @@
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
       <c r="L26" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>173</v>
       </c>
@@ -5693,10 +5715,10 @@
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>176</v>
       </c>
@@ -5723,10 +5745,10 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>179</v>
       </c>
@@ -5753,10 +5775,10 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>182</v>
       </c>
@@ -5787,10 +5809,10 @@
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>187</v>
       </c>
@@ -5821,10 +5843,10 @@
       </c>
       <c r="K31" s="3"/>
       <c r="L31" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>191</v>
       </c>
@@ -5855,10 +5877,10 @@
       </c>
       <c r="K32" s="3"/>
       <c r="L32" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>195</v>
       </c>
@@ -5889,7 +5911,7 @@
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -5909,16 +5931,16 @@
       <selection activeCell="F2" sqref="F2:F13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5935,247 +5957,247 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>297</v>
+        <v>235</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>299</v>
+        <v>237</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>300</v>
+        <v>238</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>301</v>
+        <v>239</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>302</v>
+        <v>240</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>303</v>
+        <v>241</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>304</v>
+        <v>242</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>305</v>
+        <v>243</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>306</v>
+        <v>244</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>307</v>
+        <v>245</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>308</v>
+        <v>246</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>309</v>
+        <v>247</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>310</v>
+        <v>248</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>311</v>
+        <v>249</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>312</v>
+        <v>250</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>313</v>
+        <v>251</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>314</v>
+        <v>252</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>315</v>
+        <v>253</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>316</v>
+        <v>254</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>317</v>
+        <v>255</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>318</v>
+        <v>256</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>319</v>
+        <v>257</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>320</v>
+        <v>258</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>321</v>
+        <v>259</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>322</v>
+        <v>260</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>323</v>
+        <v>261</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>324</v>
+        <v>262</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>325</v>
+        <v>263</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>326</v>
+        <v>264</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>327</v>
+        <v>265</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>328</v>
+        <v>266</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>16</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>329</v>
+        <v>267</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>330</v>
+        <v>268</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>331</v>
+        <v>269</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>298</v>
+        <v>236</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>332</v>
+        <v>270</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>333</v>
+        <v>271</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>
@@ -6192,18 +6214,18 @@
       <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.109375" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.109375" customWidth="1"/>
-    <col min="5" max="5" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.140625" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -6223,51 +6245,51 @@
         <v>6</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>289</v>
+        <v>227</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>290</v>
+        <v>228</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>291</v>
+        <v>229</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>292</v>
+        <v>230</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>293</v>
+        <v>231</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>294</v>
+        <v>232</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="3" t="s">
-        <v>295</v>
+        <v>233</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>296</v>
+        <v>234</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>352</v>
+        <v>290</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More work on DTU
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
+++ b/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10035" windowHeight="7020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10035" windowHeight="7020" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="parts" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="322">
   <si>
     <t>name</t>
   </si>
@@ -243,9 +243,6 @@
     <t>Repair Pack</t>
   </si>
   <si>
-    <t>Repair Unit</t>
-  </si>
-  <si>
     <t>Battery</t>
   </si>
   <si>
@@ -255,9 +252,6 @@
     <t>Jetpack</t>
   </si>
   <si>
-    <t>03.6-NanoRepairBots</t>
-  </si>
-  <si>
     <t>Nano RepairBots</t>
   </si>
   <si>
@@ -597,18 +591,12 @@
     <t>03.2-RepairPack</t>
   </si>
   <si>
-    <t>03.3-RepairUnit</t>
-  </si>
-  <si>
     <t>03.4-Battery</t>
   </si>
   <si>
     <t>03.5-HeavyArmor</t>
   </si>
   <si>
-    <t>0365-Jetpack</t>
-  </si>
-  <si>
     <t>03.1-Fan</t>
   </si>
   <si>
@@ -651,18 +639,9 @@
     <t>1{-energy}{yields}3{+coolant}</t>
   </si>
   <si>
-    <t>{flip}{yields}3{repair}</t>
-  </si>
-  <si>
-    <t>1{-energy}{yields}2{repair}</t>
-  </si>
-  <si>
     <t>{flip}{yields}3{+energy}</t>
   </si>
   <si>
-    <t>{flip}{yields}1{speed}</t>
-  </si>
-  <si>
     <t>3{-energy}2{-coolant}{yields}{fire}{bullets}{electricity}</t>
   </si>
   <si>
@@ -690,18 +669,9 @@
     <t>1{-coolant}{yields}10{+energy}</t>
   </si>
   <si>
-    <t>{yields}1{repair}</t>
-  </si>
-  <si>
-    <t>99{-coolant}{yields}3{wildAttack}</t>
-  </si>
-  <si>
     <t>{flip}{yields}6{+energy}</t>
   </si>
   <si>
-    <t>1{-energy}{yields}4{repair}</t>
-  </si>
-  <si>
     <t>1{damage}{yields}{wildAttack}</t>
   </si>
   <si>
@@ -984,16 +954,40 @@
     <t>textOnlyRules</t>
   </si>
   <si>
-    <t>2{temp}, {yields}1{+coolant}</t>
-  </si>
-  <si>
-    <t>4{defense}</t>
-  </si>
-  <si>
-    <t>2{space}</t>
-  </si>
-  <si>
-    <t>4{temp}, 1{-energy}{yields}4{+coolant}</t>
+    <t>03.6-Jetpack</t>
+  </si>
+  <si>
+    <t>03.14-NanoRepairBots</t>
+  </si>
+  <si>
+    <t>{flip}{yields}1{repair}</t>
+  </si>
+  <si>
+    <t>03.3-Armor</t>
+  </si>
+  <si>
+    <t>Armor</t>
+  </si>
+  <si>
+    <t>+1{speed}</t>
+  </si>
+  <si>
+    <t>+4{defense}</t>
+  </si>
+  <si>
+    <t>+2{defense}</t>
+  </si>
+  <si>
+    <t>+2{temp}, {yields}1{+coolant}</t>
+  </si>
+  <si>
+    <t>99{damage}{yields}3{wildAttack}</t>
+  </si>
+  <si>
+    <t>+2{space}</t>
+  </si>
+  <si>
+    <t>+4{temp}, 1{-energy}{yields}4{+coolant}</t>
   </si>
 </sst>
 </file>
@@ -1072,13 +1066,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
@@ -1893,8 +1888,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1932,7 +1927,7 @@
         <v>11</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -1952,13 +1947,13 @@
         <v>16</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -1978,13 +1973,13 @@
         <v>19</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -2004,13 +1999,13 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -2030,13 +2025,13 @@
         <v>23</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -2056,13 +2051,13 @@
         <v>26</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -2082,13 +2077,13 @@
         <v>29</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -2108,13 +2103,13 @@
         <v>52</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -2134,13 +2129,13 @@
         <v>54</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -2160,13 +2155,13 @@
         <v>56</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="G10" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -2186,13 +2181,13 @@
         <v>58</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -2212,18 +2207,18 @@
         <v>60</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>24</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
@@ -2235,21 +2230,21 @@
         <v>71</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>320</v>
+        <v>186</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>318</v>
       </c>
       <c r="G13" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>13</v>
@@ -2261,21 +2256,21 @@
         <v>71</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="G14" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>13</v>
@@ -2290,18 +2285,18 @@
         <v>72</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>209</v>
+        <v>312</v>
       </c>
       <c r="G15" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>191</v>
+        <v>313</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
@@ -2313,21 +2308,21 @@
         <v>71</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>210</v>
+        <v>314</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>317</v>
       </c>
       <c r="G16" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>13</v>
@@ -2339,21 +2334,21 @@
         <v>71</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>13</v>
@@ -2365,21 +2360,21 @@
         <v>71</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>321</v>
+        <v>74</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="G18" s="3" t="s">
         <v>27</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>194</v>
+        <v>310</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
@@ -2391,16 +2386,16 @@
         <v>71</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>212</v>
+        <v>75</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="G19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -2416,8 +2411,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J25"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2:G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2457,13 +2452,13 @@
         <v>10</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -2477,7 +2472,7 @@
         <v>31</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>15</v>
@@ -2486,14 +2481,14 @@
         <v>32</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>213</v>
+        <v>206</v>
       </c>
       <c r="H2" s="3"/>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -2507,7 +2502,7 @@
         <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>15</v>
@@ -2516,14 +2511,14 @@
         <v>34</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="H3" s="3"/>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>37</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2537,7 +2532,7 @@
         <v>31</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>15</v>
@@ -2546,14 +2541,14 @@
         <v>36</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>215</v>
+        <v>208</v>
       </c>
       <c r="H4" s="3"/>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2567,7 +2562,7 @@
         <v>31</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>15</v>
@@ -2576,14 +2571,14 @@
         <v>39</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>216</v>
+        <v>209</v>
       </c>
       <c r="H5" s="3"/>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2597,7 +2592,7 @@
         <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>15</v>
@@ -2606,14 +2601,14 @@
         <v>41</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>217</v>
+        <v>210</v>
       </c>
       <c r="H6" s="3"/>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="7" t="s">
         <v>24</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2627,7 +2622,7 @@
         <v>31</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>15</v>
@@ -2636,14 +2631,14 @@
         <v>44</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>42</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2657,7 +2652,7 @@
         <v>31</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>15</v>
@@ -2666,14 +2661,14 @@
         <v>46</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2687,7 +2682,7 @@
         <v>31</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>15</v>
@@ -2696,14 +2691,14 @@
         <v>49</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2717,7 +2712,7 @@
         <v>31</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>51</v>
@@ -2726,14 +2721,14 @@
         <v>62</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="H10" s="3"/>
       <c r="I10" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2747,7 +2742,7 @@
         <v>31</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>51</v>
@@ -2756,14 +2751,14 @@
         <v>64</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="H11" s="3"/>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>17</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2777,7 +2772,7 @@
         <v>31</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>51</v>
@@ -2786,14 +2781,14 @@
         <v>66</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="H12" s="3"/>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2807,7 +2802,7 @@
         <v>31</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>51</v>
@@ -2816,14 +2811,14 @@
         <v>68</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="H13" s="3"/>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>27</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2837,7 +2832,7 @@
         <v>31</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>51</v>
@@ -2846,19 +2841,19 @@
         <v>70</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>77</v>
+        <v>311</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>13</v>
@@ -2867,28 +2862,28 @@
         <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>222</v>
+        <v>312</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>13</v>
@@ -2897,28 +2892,28 @@
         <v>31</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>223</v>
+        <v>319</v>
       </c>
       <c r="H16" s="3"/>
       <c r="I16" s="3" t="s">
         <v>24</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>13</v>
@@ -2927,28 +2922,28 @@
         <v>31</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>322</v>
+        <v>80</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>320</v>
       </c>
       <c r="H17" s="3"/>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>47</v>
       </c>
       <c r="J17" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>13</v>
@@ -2957,28 +2952,28 @@
         <v>31</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="H18" s="3"/>
       <c r="I18" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J18" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
@@ -2987,28 +2982,28 @@
         <v>31</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="G19" s="3" t="s">
-        <v>321</v>
+        <v>84</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>316</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J19" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>13</v>
@@ -3017,28 +3012,28 @@
         <v>31</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>225</v>
+        <v>86</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>317</v>
       </c>
       <c r="H20" s="3"/>
-      <c r="I20" s="3" t="s">
-        <v>17</v>
+      <c r="I20" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="J20" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
@@ -3047,27 +3042,27 @@
         <v>31</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>229</v>
-      </c>
-      <c r="G21" t="s">
-        <v>323</v>
+        <v>219</v>
+      </c>
+      <c r="G21" s="6" t="s">
+        <v>321</v>
       </c>
       <c r="I21" s="3" t="s">
         <v>17</v>
       </c>
       <c r="J21" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B22" s="3" t="s">
         <v>13</v>
@@ -3076,28 +3071,28 @@
         <v>31</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>71</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>212</v>
+        <v>88</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>315</v>
       </c>
       <c r="H22" s="3"/>
       <c r="I22" s="3" t="s">
         <v>47</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>13</v>
@@ -3106,26 +3101,26 @@
         <v>31</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>231</v>
-      </c>
-      <c r="G23" s="7"/>
+        <v>221</v>
+      </c>
+      <c r="G23" s="8"/>
       <c r="H23" s="5" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="I23" s="5"/>
       <c r="J23" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>13</v>
@@ -3134,26 +3129,26 @@
         <v>31</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="7"/>
+        <v>90</v>
+      </c>
+      <c r="G24" s="8"/>
       <c r="H24" s="5" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="I24" s="5"/>
       <c r="J24" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>13</v>
@@ -3162,21 +3157,21 @@
         <v>31</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="G25" s="7"/>
+        <v>226</v>
+      </c>
+      <c r="G25" s="8"/>
       <c r="H25" s="5" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="I25" s="5"/>
       <c r="J25" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -3235,1141 +3230,1141 @@
         <v>9</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>184</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>186</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="G7" s="3"/>
       <c r="H7" s="3" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>95</v>
-      </c>
       <c r="F11" s="3" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="G19" s="3"/>
       <c r="H19" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="G37" s="3"/>
       <c r="H37" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="G39" s="3"/>
       <c r="H39" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="G40" s="2"/>
       <c r="H40" s="2" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="G41" s="3"/>
       <c r="H41" s="3" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="I41" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="G43" s="5"/>
       <c r="H43" s="5" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="I43" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
@@ -4382,8 +4377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4412,227 +4407,227 @@
         <v>6</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>239</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>249</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>261</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>251</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
checking in some changes to DTU and timmy's reading game
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
+++ b/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mike\CardGenerator\CardFormatter\Data\DefendTheUniversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A80F1132-0685-47E5-B20E-89E6DE7B5D0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2AD36-7AB5-4300-B9E6-8A0570B9F6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0.characers" sheetId="4" r:id="rId1"/>
@@ -19,8 +19,8 @@
     <sheet name="1.startParts" sheetId="8" r:id="rId4"/>
     <sheet name="1.technologies" sheetId="6" r:id="rId5"/>
     <sheet name="2.technologies" sheetId="7" r:id="rId6"/>
-    <sheet name="3.deck" sheetId="9" r:id="rId7"/>
-    <sheet name="3.technologies" sheetId="10" r:id="rId8"/>
+    <sheet name="3.technologies" sheetId="10" r:id="rId7"/>
+    <sheet name="3.deck" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="925" uniqueCount="306">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1028" uniqueCount="351">
   <si>
     <t>name</t>
   </si>
@@ -955,6 +955,141 @@
   </si>
   <si>
     <t>Save the Titanic</t>
+  </si>
+  <si>
+    <t>Temporal Clacker</t>
+  </si>
+  <si>
+    <t>Heinlein device</t>
+  </si>
+  <si>
+    <t>Ulysses Engine</t>
+  </si>
+  <si>
+    <t>Seven Minute Boots</t>
+  </si>
+  <si>
+    <t>Chronometric Coupler</t>
+  </si>
+  <si>
+    <t>playing</t>
+  </si>
+  <si>
+    <t>value1</t>
+  </si>
+  <si>
+    <t>value2</t>
+  </si>
+  <si>
+    <t>time.png</t>
+  </si>
+  <si>
+    <t>1{fire}</t>
+  </si>
+  <si>
+    <t>2{fire}</t>
+  </si>
+  <si>
+    <t>3{fire}</t>
+  </si>
+  <si>
+    <t>4{fire}</t>
+  </si>
+  <si>
+    <t>5{fire}</t>
+  </si>
+  <si>
+    <t>6{fire}</t>
+  </si>
+  <si>
+    <t>1{bullets}</t>
+  </si>
+  <si>
+    <t>2{bullets}</t>
+  </si>
+  <si>
+    <t>3{bullets}</t>
+  </si>
+  <si>
+    <t>4{bullets}</t>
+  </si>
+  <si>
+    <t>5{bullets}</t>
+  </si>
+  <si>
+    <t>6{bullets}</t>
+  </si>
+  <si>
+    <t>1{electricity}</t>
+  </si>
+  <si>
+    <t>2{electricity}</t>
+  </si>
+  <si>
+    <t>3{electricity}</t>
+  </si>
+  <si>
+    <t>4{electricity}</t>
+  </si>
+  <si>
+    <t>5{electricity}</t>
+  </si>
+  <si>
+    <t>6{electricity}</t>
+  </si>
+  <si>
+    <t>1{punch}</t>
+  </si>
+  <si>
+    <t>2{punch}</t>
+  </si>
+  <si>
+    <t>3{punch}</t>
+  </si>
+  <si>
+    <t>4{punch}</t>
+  </si>
+  <si>
+    <t>5{punch}</t>
+  </si>
+  <si>
+    <t>6{punch}</t>
+  </si>
+  <si>
+    <t>4{scratch}</t>
+  </si>
+  <si>
+    <t>5{scratch}</t>
+  </si>
+  <si>
+    <t>6{scratch}</t>
+  </si>
+  <si>
+    <t>1{scratch}</t>
+  </si>
+  <si>
+    <t>2{scratch}</t>
+  </si>
+  <si>
+    <t>3{scratch}</t>
+  </si>
+  <si>
+    <t>1{acid}</t>
+  </si>
+  <si>
+    <t>2{acid}</t>
+  </si>
+  <si>
+    <t>3{acid}</t>
+  </si>
+  <si>
+    <t>4{acid}</t>
+  </si>
+  <si>
+    <t>5{acid}</t>
+  </si>
+  <si>
+    <t>6{acid}</t>
   </si>
 </sst>
 </file>
@@ -1033,7 +1168,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1050,11 +1185,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="124">
+  <dxfs count="136">
     <dxf>
       <font>
         <b val="0"/>
@@ -1071,7 +1207,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1089,6 +1224,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1106,15 +1242,12 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
       <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1132,6 +1265,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1183,12 +1317,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1208,6 +1336,20 @@
       </font>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1226,6 +1368,23 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1242,20 +1401,6 @@
       </font>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -1271,6 +1416,189 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="1"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1305,7 +1633,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1323,6 +1650,15 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1340,15 +1676,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor indexed="65"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1400,6 +1727,12 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1417,12 +1750,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1457,6 +1784,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -3496,214 +3824,236 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E251B104-CBE0-412A-A44F-D6AC7AB1B073}" name="Table4" displayName="Table4" ref="A1:H12" totalsRowShown="0" headerRowDxfId="123" dataDxfId="122">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E251B104-CBE0-412A-A44F-D6AC7AB1B073}" name="Table4" displayName="Table4" ref="A1:H12" totalsRowShown="0" headerRowDxfId="135" dataDxfId="134">
   <autoFilter ref="A1:H12" xr:uid="{F4D468CF-18B3-498A-BC17-E745DF4CEB82}"/>
   <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{A213A786-11DA-408B-B0BC-C9BB84B9D667}" name="#"/>
     <tableColumn id="2" xr3:uid="{E94C7515-1DDC-4D81-9F94-4EF801633336}" name="cardTitle"/>
-    <tableColumn id="3" xr3:uid="{4EFE4612-27A8-46A5-8AC7-31E646CEE4AB}" name="name" dataDxfId="121">
+    <tableColumn id="3" xr3:uid="{4EFE4612-27A8-46A5-8AC7-31E646CEE4AB}" name="name" dataDxfId="133">
       <calculatedColumnFormula>CONCATENATE("0.0.",A2,"-",B2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{AC38C45A-5942-4316-AAB0-27BB36C688B9}" name="orientation" dataDxfId="120"/>
-    <tableColumn id="5" xr3:uid="{291872D0-7A9A-4162-A589-E8B3B385F5BA}" name="deck" dataDxfId="119"/>
-    <tableColumn id="6" xr3:uid="{5D7EF8C5-C441-49F2-970B-BF9D42FFB2A8}" name="title" dataDxfId="118"/>
-    <tableColumn id="7" xr3:uid="{C5CCC45C-4511-4878-ADB2-39DD6CEE530E}" name="textOnlyRules" dataDxfId="117"/>
-    <tableColumn id="8" xr3:uid="{84FC9B45-B29C-4B07-9FEE-47E29BA5B468}" name="image" dataDxfId="116"/>
+    <tableColumn id="4" xr3:uid="{AC38C45A-5942-4316-AAB0-27BB36C688B9}" name="orientation" dataDxfId="132"/>
+    <tableColumn id="5" xr3:uid="{291872D0-7A9A-4162-A589-E8B3B385F5BA}" name="deck" dataDxfId="131"/>
+    <tableColumn id="6" xr3:uid="{5D7EF8C5-C441-49F2-970B-BF9D42FFB2A8}" name="title" dataDxfId="130"/>
+    <tableColumn id="7" xr3:uid="{C5CCC45C-4511-4878-ADB2-39DD6CEE530E}" name="textOnlyRules" dataDxfId="129"/>
+    <tableColumn id="8" xr3:uid="{84FC9B45-B29C-4B07-9FEE-47E29BA5B468}" name="image" dataDxfId="128"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:AL27" totalsRowShown="0" headerRowDxfId="115" dataDxfId="113" headerRowBorderDxfId="114" tableBorderDxfId="112">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:AL27" totalsRowShown="0" headerRowDxfId="127" dataDxfId="125" headerRowBorderDxfId="126" tableBorderDxfId="124">
   <autoFilter ref="A1:AL27" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="38">
-    <tableColumn id="38" xr3:uid="{A1BAED55-EE5E-437E-BC6E-7B0DD6DDF807}" name="#" dataDxfId="111"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name" dataDxfId="110">
+    <tableColumn id="38" xr3:uid="{A1BAED55-EE5E-437E-BC6E-7B0DD6DDF807}" name="#" dataDxfId="123"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="name" dataDxfId="122">
       <calculatedColumnFormula>CONCATENATE("0.1.",A2,"-",F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="orientation" dataDxfId="109"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="deck" dataDxfId="108"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="type" dataDxfId="107" totalsRowDxfId="106"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="title" dataDxfId="105"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="f" dataDxfId="104"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="b" dataDxfId="103"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="e" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="p" dataDxfId="101"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="s" dataDxfId="100"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="a" dataDxfId="99"/>
-    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="fb" dataDxfId="98">
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="orientation" dataDxfId="121"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="deck" dataDxfId="120"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="type" dataDxfId="119" totalsRowDxfId="118"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="title" dataDxfId="117"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="f" dataDxfId="116"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="b" dataDxfId="115"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="e" dataDxfId="114"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="p" dataDxfId="113"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="s" dataDxfId="112"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="a" dataDxfId="111"/>
+    <tableColumn id="36" xr3:uid="{00000000-0010-0000-0000-000024000000}" name="fb" dataDxfId="110">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[f]]=1, Table2[[#This Row],[b]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="fe" dataDxfId="97">
+    <tableColumn id="35" xr3:uid="{00000000-0010-0000-0000-000023000000}" name="fe" dataDxfId="109">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[f]]=1, Table2[[#This Row],[e]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="fp" dataDxfId="96">
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="fp" dataDxfId="108">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[f]]=1, Table2[[#This Row],[p]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="fs" dataDxfId="95">
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="fs" dataDxfId="107">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[f]]=1, Table2[[#This Row],[s]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="fa" dataDxfId="94">
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="fa" dataDxfId="106">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[f]]=1, Table2[[#This Row],[a]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="be" dataDxfId="93">
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="be" dataDxfId="105">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[b]]=1, Table2[[#This Row],[e]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="bp" dataDxfId="92">
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="bp" dataDxfId="104">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[b]]=1, Table2[[#This Row],[p]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="bs" dataDxfId="91">
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="bs" dataDxfId="103">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[b]]=1, Table2[[#This Row],[s]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ba" dataDxfId="90">
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="ba" dataDxfId="102">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[b]]=1, Table2[[#This Row],[a]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ep" dataDxfId="89">
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="ep" dataDxfId="101">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[e]]=1, Table2[[#This Row],[p]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="es" dataDxfId="88">
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="es" dataDxfId="100">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[e]]=1, Table2[[#This Row],[s]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="ea" dataDxfId="87">
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="ea" dataDxfId="99">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[e]]=1, Table2[[#This Row],[a]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ps" dataDxfId="86">
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="ps" dataDxfId="98">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[p]]=1, Table2[[#This Row],[s]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="pa" dataDxfId="85">
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="pa" dataDxfId="97">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[p]]=1, Table2[[#This Row],[a]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="sa" dataDxfId="84">
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="sa" dataDxfId="96">
       <calculatedColumnFormula>IF(AND(Table2[[#This Row],[s]]=1, Table2[[#This Row],[a]]=1), 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Fire" dataDxfId="83" totalsRowDxfId="82">
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Fire" dataDxfId="95" totalsRowDxfId="94">
       <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[f]]), "", "{fire}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Bullets" dataDxfId="81" totalsRowDxfId="80">
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Bullets" dataDxfId="93" totalsRowDxfId="92">
       <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[b]]), "", "{bullets}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Electricity" dataDxfId="79" totalsRowDxfId="78">
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Electricity" dataDxfId="91" totalsRowDxfId="90">
       <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[e]]), "", "{electricity}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Punch" dataDxfId="77" totalsRowDxfId="76">
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Punch" dataDxfId="89" totalsRowDxfId="88">
       <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[p]]), "", "{punch}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Scratch" dataDxfId="75" totalsRowDxfId="74">
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Scratch" dataDxfId="87" totalsRowDxfId="86">
       <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[s]]), "", "{scratch}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Acid" dataDxfId="73" totalsRowDxfId="72">
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Acid" dataDxfId="85" totalsRowDxfId="84">
       <calculatedColumnFormula>IF(ISBLANK(Table2[[#This Row],[a]]), "", "{acid}")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="requirements" dataDxfId="71">
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="requirements" dataDxfId="83">
       <calculatedColumnFormula>TRIM(CONCATENATE(IF(Table2[[#This Row],[f]]=1,"{fire} ",""),IF(Table2[[#This Row],[b]]=1,"{bullets} ",""),IF(Table2[[#This Row],[e]]=1,"{electricity} ",""),IF(Table2[[#This Row],[p]]=1,"{punch} ",""),IF(Table2[[#This Row],[s]]=1,"{scratch} ",""),IF(Table2[[#This Row],[a]]=1,"{acid} ","")))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="bonusAbilities" dataDxfId="70"/>
-    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="health" dataDxfId="69"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="effects" dataDxfId="68"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="image" dataDxfId="67"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="bonusAbilities" dataDxfId="82"/>
+    <tableColumn id="37" xr3:uid="{00000000-0010-0000-0000-000025000000}" name="health" dataDxfId="81"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="effects" dataDxfId="80"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="image" dataDxfId="79"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="B1:I19" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="B1:I19" totalsRowShown="0" headerRowDxfId="78" dataDxfId="76" headerRowBorderDxfId="77" tableBorderDxfId="75">
   <autoFilter ref="B1:I19" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="name" dataDxfId="62">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="name" dataDxfId="74">
       <calculatedColumnFormula>CONCATENATE("1.0.",A2,"-",F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="orientation" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="deck" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="type" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="title" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="rules" dataDxfId="57"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="size" dataDxfId="56"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="image" dataDxfId="55"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="orientation" dataDxfId="73"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="deck" dataDxfId="72"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="type" dataDxfId="71"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="title" dataDxfId="70"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="rules" dataDxfId="69"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="size" dataDxfId="68"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0100-00000A000000}" name="image" dataDxfId="67"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FE5F990D-4CD4-47BF-89CE-9D9DB7D92DE7}" name="Table17" displayName="Table17" ref="B1:I6" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{FE5F990D-4CD4-47BF-89CE-9D9DB7D92DE7}" name="Table17" displayName="Table17" ref="B1:I6" totalsRowShown="0" headerRowDxfId="66" dataDxfId="64" headerRowBorderDxfId="65" tableBorderDxfId="63">
   <autoFilter ref="B1:I6" xr:uid="{817495A5-F131-4B12-9376-A2205CF811DF}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{9D8DDAD7-DC55-44C8-85DB-C568161F5914}" name="name" dataDxfId="50">
+    <tableColumn id="1" xr3:uid="{9D8DDAD7-DC55-44C8-85DB-C568161F5914}" name="name" dataDxfId="62">
       <calculatedColumnFormula>CONCATENATE("1.1.",A2,"-",F2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5298D532-3C61-4924-8774-2A347E08B6FF}" name="orientation" dataDxfId="49"/>
-    <tableColumn id="3" xr3:uid="{8FF06403-FC8D-41EC-9050-518E8AA5047F}" name="deck" dataDxfId="48"/>
-    <tableColumn id="4" xr3:uid="{263B1478-94D8-4FAB-A2B8-92732B6B797B}" name="type" dataDxfId="47"/>
-    <tableColumn id="5" xr3:uid="{BB70B060-0409-47F5-A752-969E92EF995E}" name="title" dataDxfId="46"/>
-    <tableColumn id="6" xr3:uid="{39B568A2-E907-4E0F-A927-AF3600CD1725}" name="rules" dataDxfId="45"/>
-    <tableColumn id="9" xr3:uid="{450CFC51-86AB-4AF5-8A18-010848DE01AB}" name="size" dataDxfId="44"/>
-    <tableColumn id="10" xr3:uid="{0CE46F9C-3775-479D-9973-F70504A89D2F}" name="image" dataDxfId="43"/>
+    <tableColumn id="2" xr3:uid="{5298D532-3C61-4924-8774-2A347E08B6FF}" name="orientation" dataDxfId="61"/>
+    <tableColumn id="3" xr3:uid="{8FF06403-FC8D-41EC-9050-518E8AA5047F}" name="deck" dataDxfId="60"/>
+    <tableColumn id="4" xr3:uid="{263B1478-94D8-4FAB-A2B8-92732B6B797B}" name="type" dataDxfId="59"/>
+    <tableColumn id="5" xr3:uid="{BB70B060-0409-47F5-A752-969E92EF995E}" name="title" dataDxfId="58"/>
+    <tableColumn id="6" xr3:uid="{39B568A2-E907-4E0F-A927-AF3600CD1725}" name="rules" dataDxfId="57"/>
+    <tableColumn id="9" xr3:uid="{450CFC51-86AB-4AF5-8A18-010848DE01AB}" name="size" dataDxfId="56"/>
+    <tableColumn id="10" xr3:uid="{0CE46F9C-3775-479D-9973-F70504A89D2F}" name="image" dataDxfId="55"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:K21" totalsRowShown="0" headerRowDxfId="42" dataDxfId="40" headerRowBorderDxfId="41" tableBorderDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table3" displayName="Table3" ref="A1:K21" totalsRowShown="0" headerRowDxfId="54" dataDxfId="52" headerRowBorderDxfId="53" tableBorderDxfId="51">
   <autoFilter ref="A1:K21" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <tableColumns count="11">
-    <tableColumn id="9" xr3:uid="{7226E313-BE2D-44C9-8533-17F669E45651}" name="#" dataDxfId="38"/>
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="name" dataDxfId="37">
+    <tableColumn id="9" xr3:uid="{7226E313-BE2D-44C9-8533-17F669E45651}" name="#" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="name" dataDxfId="49">
       <calculatedColumnFormula>CONCATENATE("1.2.",A2,"-",G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="orientation" dataDxfId="36"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="deck" dataDxfId="35"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="costs" dataDxfId="34"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="type" dataDxfId="33"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="title" dataDxfId="32"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="rules" dataDxfId="31"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="textOnlyRules" dataDxfId="30"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="size" dataDxfId="29"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="image" dataDxfId="28"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="orientation" dataDxfId="48"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="deck" dataDxfId="47"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="costs" dataDxfId="46"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0200-000006000000}" name="type" dataDxfId="45"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0200-000007000000}" name="title" dataDxfId="44"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0200-000008000000}" name="rules" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="textOnlyRules" dataDxfId="42"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0200-00000C000000}" name="size" dataDxfId="41"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0200-00000D000000}" name="image" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5FF89812-FDBF-490E-A305-F7C856C5ADC6}" name="Table36" displayName="Table36" ref="A1:J21" totalsRowShown="0" headerRowDxfId="27" dataDxfId="25" headerRowBorderDxfId="26" tableBorderDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5FF89812-FDBF-490E-A305-F7C856C5ADC6}" name="Table36" displayName="Table36" ref="A1:J21" totalsRowShown="0" headerRowDxfId="39" dataDxfId="37" headerRowBorderDxfId="38" tableBorderDxfId="36">
   <autoFilter ref="A1:J21" xr:uid="{1188DE45-EC46-4A93-B352-55701A900BAA}"/>
   <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{E25695D3-2C65-4873-BAF0-00ABEDEBA956}" name="#" dataDxfId="23"/>
-    <tableColumn id="1" xr3:uid="{89A5AC31-5E81-49C0-946A-084D3E82D05B}" name="name" dataDxfId="14">
+    <tableColumn id="9" xr3:uid="{E25695D3-2C65-4873-BAF0-00ABEDEBA956}" name="#" dataDxfId="35"/>
+    <tableColumn id="1" xr3:uid="{89A5AC31-5E81-49C0-946A-084D3E82D05B}" name="name" dataDxfId="34">
       <calculatedColumnFormula>CONCATENATE("2.0.",A2,"-",G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{5DC33A9D-A50A-4D20-BE24-7650F75F0E91}" name="orientation" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{3C1A3176-2407-4332-BC37-51A350252AE4}" name="deck" dataDxfId="21"/>
-    <tableColumn id="5" xr3:uid="{9EAD9436-E5DB-49C7-B324-61E5443D8B6D}" name="costs" dataDxfId="20"/>
-    <tableColumn id="6" xr3:uid="{84C40A88-F1E5-4DFD-8C49-9F2581518EE4}" name="type" dataDxfId="19"/>
-    <tableColumn id="7" xr3:uid="{81A5CA9B-EF59-41B1-B133-4AA56FA843C5}" name="title" dataDxfId="18"/>
-    <tableColumn id="8" xr3:uid="{FFB9C408-A9E6-44CE-925E-2AA944394E8A}" name="rules" dataDxfId="17"/>
-    <tableColumn id="4" xr3:uid="{438FED7D-64B5-44D1-BA52-33DF37240C6F}" name="textOnlyRules" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{23619D43-5F2D-4830-8406-1F26807F8854}" name="image" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{5DC33A9D-A50A-4D20-BE24-7650F75F0E91}" name="orientation" dataDxfId="33"/>
+    <tableColumn id="3" xr3:uid="{3C1A3176-2407-4332-BC37-51A350252AE4}" name="deck" dataDxfId="32"/>
+    <tableColumn id="5" xr3:uid="{9EAD9436-E5DB-49C7-B324-61E5443D8B6D}" name="costs" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{84C40A88-F1E5-4DFD-8C49-9F2581518EE4}" name="type" dataDxfId="30"/>
+    <tableColumn id="7" xr3:uid="{81A5CA9B-EF59-41B1-B133-4AA56FA843C5}" name="title" dataDxfId="29"/>
+    <tableColumn id="8" xr3:uid="{FFB9C408-A9E6-44CE-925E-2AA944394E8A}" name="rules" dataDxfId="28"/>
+    <tableColumn id="4" xr3:uid="{438FED7D-64B5-44D1-BA52-33DF37240C6F}" name="textOnlyRules" dataDxfId="27"/>
+    <tableColumn id="13" xr3:uid="{23619D43-5F2D-4830-8406-1F26807F8854}" name="image" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15179202-3318-42A9-91BC-2AAFE76E00B7}" name="Table368" displayName="Table368" ref="A1:J21" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowBorderDxfId="10" tableBorderDxfId="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{15179202-3318-42A9-91BC-2AAFE76E00B7}" name="Table368" displayName="Table368" ref="A1:J21" totalsRowShown="0" headerRowDxfId="25" dataDxfId="23" headerRowBorderDxfId="24" tableBorderDxfId="22">
   <autoFilter ref="A1:J21" xr:uid="{B96485E0-B43C-46A4-AD8C-F933F606B734}"/>
   <tableColumns count="10">
-    <tableColumn id="9" xr3:uid="{0E1AE489-89D2-49FB-AC67-C3B4C2A6529E}" name="#" dataDxfId="9"/>
-    <tableColumn id="1" xr3:uid="{ABCBCA48-BC68-468C-84EA-3FC6CAB7676B}" name="name" dataDxfId="0">
+    <tableColumn id="9" xr3:uid="{0E1AE489-89D2-49FB-AC67-C3B4C2A6529E}" name="#" dataDxfId="21"/>
+    <tableColumn id="1" xr3:uid="{ABCBCA48-BC68-468C-84EA-3FC6CAB7676B}" name="name" dataDxfId="20">
       <calculatedColumnFormula>CONCATENATE("3.1.",A2,"-",G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{4A5773D8-B818-4AC7-8B9D-E639524394EA}" name="orientation" dataDxfId="8"/>
-    <tableColumn id="3" xr3:uid="{A1544B09-AD3E-481B-A1CB-3207AFC6D425}" name="deck" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{7D2E29FC-D030-464A-B6FF-80B6311B3FF7}" name="costs" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{F3E4A2BC-C98C-44D9-8826-029A71FD4253}" name="type" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{3342924B-36D2-4B69-A971-731E1BA51773}" name="title" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{C1840625-25AD-491C-8342-FC947E7DE731}" name="rules" dataDxfId="3"/>
-    <tableColumn id="4" xr3:uid="{65BF91CC-D6DE-472D-864A-8EABE2E8316C}" name="textOnlyRules" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{46E2CA09-9EBA-424C-93B1-4EFC4E60153F}" name="image" dataDxfId="1"/>
+    <tableColumn id="2" xr3:uid="{4A5773D8-B818-4AC7-8B9D-E639524394EA}" name="orientation" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{A1544B09-AD3E-481B-A1CB-3207AFC6D425}" name="deck" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{7D2E29FC-D030-464A-B6FF-80B6311B3FF7}" name="costs" dataDxfId="17"/>
+    <tableColumn id="6" xr3:uid="{F3E4A2BC-C98C-44D9-8826-029A71FD4253}" name="type" dataDxfId="16"/>
+    <tableColumn id="7" xr3:uid="{3342924B-36D2-4B69-A971-731E1BA51773}" name="title" dataDxfId="15"/>
+    <tableColumn id="8" xr3:uid="{C1840625-25AD-491C-8342-FC947E7DE731}" name="rules" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{65BF91CC-D6DE-472D-864A-8EABE2E8316C}" name="textOnlyRules" dataDxfId="13"/>
+    <tableColumn id="13" xr3:uid="{46E2CA09-9EBA-424C-93B1-4EFC4E60153F}" name="image" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5F41DED-EC40-4BF9-9C6C-4AF8A4A74E77}" name="Table3689" displayName="Table3689" ref="A1:H19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9">
+  <autoFilter ref="A1:H19" xr:uid="{B5F41DED-EC40-4BF9-9C6C-4AF8A4A74E77}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H19">
+    <sortCondition ref="A1:A19"/>
+  </sortState>
+  <tableColumns count="8">
+    <tableColumn id="9" xr3:uid="{40A52EF8-5BEF-473E-B6AC-ECC3CCB61F1B}" name="#" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{80B31D76-F45D-4AB0-8244-20A7E6F034D3}" name="name" dataDxfId="3">
+      <calculatedColumnFormula>CONCATENATE("3.2.",A2,"-",G2)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{3A67302A-4C79-4467-B7A3-21EA389AE2C0}" name="orientation" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{10C56FF7-E440-4E90-BE15-5BFDAE784D12}" name="deck" dataDxfId="4"/>
+    <tableColumn id="5" xr3:uid="{D1E89648-2369-4EB3-A636-E980409C5939}" name="value1" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{5B4489CE-B1E5-494D-AB87-D523473E06FD}" name="value2" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{39527004-F9A7-4F5C-99EA-0FC93E792942}" name="title" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{2CCF48F2-8148-4429-B1FC-9D6DF84492BA}" name="image" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4350,7 +4700,7 @@
   <dimension ref="A1:AL27"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AL28" sqref="AL28"/>
+      <selection activeCell="AH27" sqref="AH27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7944,7 +8294,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13:I19"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9488,7 +9838,7 @@
   <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="A1:J21"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10172,23 +10522,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF6E018-AD1D-4BFD-9424-9832D8579396}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{271F8292-29A7-4472-A92A-E8F682A8CC90}">
   <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10678,7 +11016,7 @@
       </c>
       <c r="B17" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>3.1.15-</v>
+        <v>3.1.15-Temporal Clacker</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>11</v>
@@ -10692,7 +11030,9 @@
       <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5" t="s">
+        <v>306</v>
+      </c>
       <c r="H17" s="8"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
@@ -10705,7 +11045,7 @@
       </c>
       <c r="B18" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>3.1.16-</v>
+        <v>3.1.16-Heinlein device</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>11</v>
@@ -10719,7 +11059,9 @@
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="5" t="s">
+        <v>307</v>
+      </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="5" t="s">
@@ -10732,7 +11074,7 @@
       </c>
       <c r="B19" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>3.1.17-</v>
+        <v>3.1.17-Ulysses Engine</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>11</v>
@@ -10746,7 +11088,9 @@
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5" t="s">
+        <v>308</v>
+      </c>
       <c r="H19" s="8"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
@@ -10759,7 +11103,7 @@
       </c>
       <c r="B20" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>3.1.18-</v>
+        <v>3.1.18-Chronometric Coupler</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>11</v>
@@ -10773,7 +11117,9 @@
       <c r="F20" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="5" t="s">
+        <v>310</v>
+      </c>
       <c r="H20" s="8"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
@@ -10786,7 +11132,7 @@
       </c>
       <c r="B21" s="8" t="str">
         <f t="shared" si="0"/>
-        <v>3.1.19-</v>
+        <v>3.1.19-Seven Minute Boots</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>11</v>
@@ -10800,7 +11146,9 @@
       <c r="F21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G21" s="15"/>
+      <c r="G21" s="15" t="s">
+        <v>309</v>
+      </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="5" t="s">
@@ -10814,4 +11162,509 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF6E018-AD1D-4BFD-9424-9832D8579396}">
+  <dimension ref="A1:H19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O15" sqref="O15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="16" width="11.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
+        <v>208</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="str">
+        <f>CONCATENATE("3.2.",A2,"-",G2)</f>
+        <v>3.2.0-</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" t="s">
+        <v>315</v>
+      </c>
+      <c r="F2" t="s">
+        <v>322</v>
+      </c>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="8">
+        <v>1</v>
+      </c>
+      <c r="B3" s="8" t="str">
+        <f>CONCATENATE("3.2.",A3,"-",G3)</f>
+        <v>3.2.1-</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="G3" s="5"/>
+      <c r="H3" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="8">
+        <v>2</v>
+      </c>
+      <c r="B4" s="8" t="str">
+        <f>CONCATENATE("3.2.",A4,"-",G4)</f>
+        <v>3.2.2-</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E4" t="s">
+        <v>317</v>
+      </c>
+      <c r="F4" t="s">
+        <v>336</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>3</v>
+      </c>
+      <c r="B5" s="8" t="str">
+        <f>CONCATENATE("3.2.",A5,"-",G5)</f>
+        <v>3.2.3-</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E5" t="s">
+        <v>318</v>
+      </c>
+      <c r="F5" t="s">
+        <v>340</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>4</v>
+      </c>
+      <c r="B6" s="8" t="str">
+        <f>CONCATENATE("3.2.",A6,"-",G6)</f>
+        <v>3.2.4-</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E6" t="s">
+        <v>319</v>
+      </c>
+      <c r="F6" t="s">
+        <v>350</v>
+      </c>
+      <c r="G6" s="5"/>
+      <c r="H6" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="8">
+        <v>5</v>
+      </c>
+      <c r="B7" s="8" t="str">
+        <f>CONCATENATE("3.2.",A7,"-",G7)</f>
+        <v>3.2.5-</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="8">
+        <v>6</v>
+      </c>
+      <c r="B8" s="8" t="str">
+        <f>CONCATENATE("3.2.",A8,"-",G8)</f>
+        <v>3.2.6-</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="8">
+        <v>7</v>
+      </c>
+      <c r="B9" s="8" t="str">
+        <f>CONCATENATE("3.2.",A9,"-",G9)</f>
+        <v>3.2.7-</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="G9" s="5"/>
+      <c r="H9" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="8">
+        <v>8</v>
+      </c>
+      <c r="B10" s="8" t="str">
+        <f>CONCATENATE("3.2.",A10,"-",G10)</f>
+        <v>3.2.8-</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E10" t="s">
+        <v>325</v>
+      </c>
+      <c r="F10" t="s">
+        <v>342</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="8">
+        <v>9</v>
+      </c>
+      <c r="B11" s="8" t="str">
+        <f>CONCATENATE("3.2.",A11,"-",G11)</f>
+        <v>3.2.9-</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E11" t="s">
+        <v>326</v>
+      </c>
+      <c r="F11" t="s">
+        <v>346</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="8">
+        <v>10</v>
+      </c>
+      <c r="B12" s="8" t="str">
+        <f>CONCATENATE("3.2.",A12,"-",G12)</f>
+        <v>3.2.10-</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E12" t="s">
+        <v>327</v>
+      </c>
+      <c r="F12" t="s">
+        <v>348</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="8">
+        <v>11</v>
+      </c>
+      <c r="B13" s="8" t="str">
+        <f>CONCATENATE("3.2.",A13,"-",G13)</f>
+        <v>3.2.11-</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E13" t="s">
+        <v>328</v>
+      </c>
+      <c r="F13" t="s">
+        <v>337</v>
+      </c>
+      <c r="G13" s="5"/>
+      <c r="H13" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="8">
+        <v>12</v>
+      </c>
+      <c r="B14" s="8" t="str">
+        <f>CONCATENATE("3.2.",A14,"-",G14)</f>
+        <v>3.2.12-</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>341</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="8">
+        <v>13</v>
+      </c>
+      <c r="B15" s="8" t="str">
+        <f>CONCATENATE("3.2.",A15,"-",G15)</f>
+        <v>3.2.13-</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="F15" t="s">
+        <v>347</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="8">
+        <v>14</v>
+      </c>
+      <c r="B16" s="8" t="str">
+        <f>CONCATENATE("3.2.",A16,"-",G16)</f>
+        <v>3.2.14-</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E16" t="s">
+        <v>333</v>
+      </c>
+      <c r="F16" t="s">
+        <v>344</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="8">
+        <v>15</v>
+      </c>
+      <c r="B17" s="8" t="str">
+        <f>CONCATENATE("3.2.",A17,"-",G17)</f>
+        <v>3.2.15-</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E17" t="s">
+        <v>334</v>
+      </c>
+      <c r="F17" t="s">
+        <v>339</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="8">
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="str">
+        <f>CONCATENATE("3.2.",A18,"-",G18)</f>
+        <v>3.2.16-</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="G18" s="5"/>
+      <c r="H18" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="8">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8" t="str">
+        <f>CONCATENATE("3.2.",A19,"-",G19)</f>
+        <v>3.2.17-</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="E19" s="16" t="s">
+        <v>343</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
last changes on old compy
</commit_message>
<xml_diff>
--- a/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
+++ b/CardFormatter/Data/DefendTheUniversity/DataFile.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Mike\CardGenerator\CardFormatter\Data\DefendTheUniversity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15D2AD36-7AB5-4300-B9E6-8A0570B9F6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACD51846-7E50-4229-BCF7-84A53635F379}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="0.characers" sheetId="4" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <t>Fury Beast</t>
   </si>
   <si>
-    <t>Berthaly</t>
-  </si>
-  <si>
     <t>Megasaur</t>
   </si>
   <si>
@@ -1090,6 +1087,9 @@
   </si>
   <si>
     <t>6{acid}</t>
+  </si>
+  <si>
+    <t>Mycetozoa</t>
   </si>
 </sst>
 </file>
@@ -1242,12 +1242,6 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="0" tint="-0.14999847407452621"/>
-          <bgColor theme="0" tint="-0.14999847407452621"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1265,7 +1259,12 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="0" tint="-0.14999847407452621"/>
+          <bgColor theme="0" tint="-0.14999847407452621"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <font>
@@ -1317,6 +1316,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <font>
@@ -1337,13 +1337,6 @@
     </dxf>
     <dxf>
       <border outline="0">
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
         <top style="thin">
           <color theme="1"/>
         </top>
@@ -1365,6 +1358,13 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="1"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -4038,20 +4038,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5F41DED-EC40-4BF9-9C6C-4AF8A4A74E77}" name="Table3689" displayName="Table3689" ref="A1:H19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10" headerRowBorderDxfId="8" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{B5F41DED-EC40-4BF9-9C6C-4AF8A4A74E77}" name="Table3689" displayName="Table3689" ref="A1:H19" totalsRowShown="0" headerRowDxfId="11" dataDxfId="9" headerRowBorderDxfId="10" tableBorderDxfId="8">
   <autoFilter ref="A1:H19" xr:uid="{B5F41DED-EC40-4BF9-9C6C-4AF8A4A74E77}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H19">
     <sortCondition ref="A1:A19"/>
   </sortState>
   <tableColumns count="8">
     <tableColumn id="9" xr3:uid="{40A52EF8-5BEF-473E-B6AC-ECC3CCB61F1B}" name="#" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{80B31D76-F45D-4AB0-8244-20A7E6F034D3}" name="name" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{80B31D76-F45D-4AB0-8244-20A7E6F034D3}" name="name" dataDxfId="6">
       <calculatedColumnFormula>CONCATENATE("3.2.",A2,"-",G2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{3A67302A-4C79-4467-B7A3-21EA389AE2C0}" name="orientation" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{3A67302A-4C79-4467-B7A3-21EA389AE2C0}" name="orientation" dataDxfId="5"/>
     <tableColumn id="3" xr3:uid="{10C56FF7-E440-4E90-BE15-5BFDAE784D12}" name="deck" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{D1E89648-2369-4EB3-A636-E980409C5939}" name="value1" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{5B4489CE-B1E5-494D-AB87-D523473E06FD}" name="value2" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D1E89648-2369-4EB3-A636-E980409C5939}" name="value1" dataDxfId="3"/>
+    <tableColumn id="6" xr3:uid="{5B4489CE-B1E5-494D-AB87-D523473E06FD}" name="value2" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{39527004-F9A7-4F5C-99EA-0FC93E792942}" name="title" dataDxfId="1"/>
     <tableColumn id="13" xr3:uid="{2CCF48F2-8148-4429-B1FC-9D6DF84492BA}" name="image" dataDxfId="0"/>
   </tableColumns>
@@ -4364,10 +4364,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B1" t="s">
         <v>208</v>
-      </c>
-      <c r="B1" t="s">
-        <v>209</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -4382,7 +4382,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>66</v>
@@ -4393,7 +4393,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C2" t="str">
         <f>CONCATENATE("0.0.",A2,"-",B2)</f>
@@ -4406,13 +4406,13 @@
         <v>65</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -4420,7 +4420,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C3" t="str">
         <f t="shared" ref="C3:C12" si="0">CONCATENATE("0.0.",A3,"-",B3)</f>
@@ -4433,13 +4433,13 @@
         <v>65</v>
       </c>
       <c r="F3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -4447,7 +4447,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C4" t="str">
         <f t="shared" si="0"/>
@@ -4460,13 +4460,13 @@
         <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -4474,7 +4474,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -4487,13 +4487,13 @@
         <v>65</v>
       </c>
       <c r="F5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="H5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -4501,7 +4501,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -4514,13 +4514,13 @@
         <v>65</v>
       </c>
       <c r="F6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -4528,7 +4528,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -4541,13 +4541,13 @@
         <v>65</v>
       </c>
       <c r="F7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -4555,7 +4555,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -4568,13 +4568,13 @@
         <v>65</v>
       </c>
       <c r="F8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H8" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -4582,7 +4582,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -4595,13 +4595,13 @@
         <v>65</v>
       </c>
       <c r="F9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="H9" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -4609,7 +4609,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -4622,13 +4622,13 @@
         <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G10" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -4636,7 +4636,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
@@ -4649,13 +4649,13 @@
         <v>65</v>
       </c>
       <c r="F11" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G11" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="H11" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -4663,7 +4663,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -4676,13 +4676,13 @@
         <v>65</v>
       </c>
       <c r="F12" t="s">
+        <v>116</v>
+      </c>
+      <c r="G12" t="s">
         <v>117</v>
       </c>
-      <c r="G12" t="s">
-        <v>118</v>
-      </c>
       <c r="H12" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -4699,8 +4699,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AL27"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AH27" sqref="AH27"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4725,7 +4725,7 @@
   <sheetData>
     <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -4743,85 +4743,85 @@
         <v>5</v>
       </c>
       <c r="G1" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>156</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="4" t="s">
         <v>157</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="M1" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="M1" s="4" t="s">
+      <c r="N1" s="4" t="s">
         <v>159</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>160</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="4" t="s">
         <v>162</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="T1" s="4" t="s">
+      <c r="U1" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="V1" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="W1" s="4" t="s">
         <v>168</v>
       </c>
-      <c r="W1" s="4" t="s">
+      <c r="X1" s="4" t="s">
         <v>169</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="Y1" s="4" t="s">
+      <c r="Z1" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="4" t="s">
         <v>172</v>
       </c>
-      <c r="AA1" s="4" t="s">
-        <v>173</v>
-      </c>
       <c r="AB1" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AC1" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>148</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="AG1" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="AH1" s="4" t="s">
         <v>6</v>
@@ -4830,7 +4830,7 @@
         <v>7</v>
       </c>
       <c r="AJ1" s="4" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AK1" s="4" t="s">
         <v>8</v>
@@ -4848,13 +4848,13 @@
         <v>0.1.0-Leviathan</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="10" t="s">
         <v>57</v>
@@ -4957,13 +4957,13 @@
       </c>
       <c r="AI2" s="10"/>
       <c r="AJ2" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK2" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL2" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
@@ -4975,13 +4975,13 @@
         <v>0.1.1-Cloudshark</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="10" t="s">
         <v>56</v>
@@ -5084,13 +5084,13 @@
       </c>
       <c r="AI3" s="10"/>
       <c r="AJ3" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK3" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL3" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -5102,13 +5102,13 @@
         <v>0.1.2-Scout</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>60</v>
@@ -5211,13 +5211,13 @@
       </c>
       <c r="AI4" s="10"/>
       <c r="AJ4" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK4" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL4" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -5229,13 +5229,13 @@
         <v>0.1.3-Puffer</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>58</v>
@@ -5338,13 +5338,13 @@
       </c>
       <c r="AI5" s="10"/>
       <c r="AJ5" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK5" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL5" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
@@ -5356,16 +5356,16 @@
         <v>0.1.4-Zombie</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -5465,13 +5465,13 @@
       </c>
       <c r="AI6" s="10"/>
       <c r="AJ6" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK6" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL6" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -5483,13 +5483,13 @@
         <v>0.1.5-Land Kraken</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="10" t="s">
         <v>59</v>
@@ -5592,13 +5592,13 @@
       </c>
       <c r="AI7" s="10"/>
       <c r="AJ7" s="10" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="AK7" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="AL7" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
@@ -5610,13 +5610,13 @@
         <v>0.1.6-Fury Beast</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="10" t="s">
         <v>68</v>
@@ -5721,13 +5721,13 @@
       </c>
       <c r="AI8" s="10"/>
       <c r="AJ8" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AK8" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AL8" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
@@ -5739,13 +5739,13 @@
         <v>0.1.7-Animalcular Cloud</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>67</v>
@@ -5850,13 +5850,13 @@
       </c>
       <c r="AI9" s="10"/>
       <c r="AJ9" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AK9" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AL9" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
@@ -5868,13 +5868,13 @@
         <v>0.1.8-Berserker</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="10" t="s">
         <v>63</v>
@@ -5979,13 +5979,13 @@
       </c>
       <c r="AI10" s="10"/>
       <c r="AJ10" s="10" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="AK10" s="10" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AL10" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
@@ -5997,13 +5997,13 @@
         <v>0.1.9-Mycohemoth</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="10" t="s">
         <v>55</v>
@@ -6110,13 +6110,13 @@
       </c>
       <c r="AI11" s="10"/>
       <c r="AJ11" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK11" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL11" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:38" x14ac:dyDescent="0.25">
@@ -6128,16 +6128,16 @@
         <v>0.1.10-Daidarabotchi</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G12" s="10">
         <v>1</v>
@@ -6241,13 +6241,13 @@
       </c>
       <c r="AI12" s="10"/>
       <c r="AJ12" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK12" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL12" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:38" x14ac:dyDescent="0.25">
@@ -6259,16 +6259,16 @@
         <v>0.1.11-Megasaur</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" s="10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10">
@@ -6372,13 +6372,13 @@
       </c>
       <c r="AI13" s="10"/>
       <c r="AJ13" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK13" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL13" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="14" spans="1:38" x14ac:dyDescent="0.25">
@@ -6390,13 +6390,13 @@
         <v>0.1.12-Hydra</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F14" s="10" t="s">
         <v>64</v>
@@ -6503,13 +6503,13 @@
       </c>
       <c r="AI14" s="10"/>
       <c r="AJ14" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK14" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL14" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:38" x14ac:dyDescent="0.25">
@@ -6521,13 +6521,13 @@
         <v>0.1.13-Aurelia Optirapax</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>61</v>
@@ -6634,13 +6634,13 @@
       </c>
       <c r="AI15" s="10"/>
       <c r="AJ15" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK15" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL15" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:38" x14ac:dyDescent="0.25">
@@ -6652,13 +6652,13 @@
         <v>0.1.14-Killbot</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F16" s="10" t="s">
         <v>54</v>
@@ -6765,13 +6765,13 @@
       </c>
       <c r="AI16" s="10"/>
       <c r="AJ16" s="10" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="AK16" s="10" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="AL16" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="17" spans="1:38" x14ac:dyDescent="0.25">
@@ -6783,16 +6783,16 @@
         <v>0.1.15-Milorg</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="G17" s="10">
         <v>1</v>
@@ -6897,16 +6897,16 @@
         <v>{fire} {punch} {scratch} {acid}</v>
       </c>
       <c r="AI17" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AJ17" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AK17" s="10" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="AL17" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="18" spans="1:38" x14ac:dyDescent="0.25">
@@ -6918,13 +6918,13 @@
         <v>0.1.16-Shambler</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>62</v>
@@ -7032,16 +7032,16 @@
         <v>{bullets} {electricity} {punch} {scratch}</v>
       </c>
       <c r="AI18" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AJ18" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AK18" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AL18" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="19" spans="1:38" x14ac:dyDescent="0.25">
@@ -7053,16 +7053,16 @@
         <v>0.1.17-Gigantanulon</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G19" s="10">
         <v>1</v>
@@ -7167,16 +7167,16 @@
         <v>{fire} {bullets} {electricity} {acid}</v>
       </c>
       <c r="AI19" s="10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="AJ19" s="10" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="AK19" s="10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="AL19" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="20" spans="1:38" x14ac:dyDescent="0.25">
@@ -7185,19 +7185,19 @@
       </c>
       <c r="B20" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>0.1.18-Berthaly</v>
+        <v>0.1.18-Mycetozoa</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>69</v>
+        <v>350</v>
       </c>
       <c r="G20" s="10"/>
       <c r="H20" s="10">
@@ -7304,16 +7304,16 @@
         <v>{bullets} {electricity} {punch} {scratch} {acid}</v>
       </c>
       <c r="AI20" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ20" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK20" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL20" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="21" spans="1:38" x14ac:dyDescent="0.25">
@@ -7325,16 +7325,16 @@
         <v>0.1.19-Rokap</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G21" s="10">
         <v>1</v>
@@ -7441,16 +7441,16 @@
         <v>{fire} {electricity} {punch} {scratch} {acid}</v>
       </c>
       <c r="AI21" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ21" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK21" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL21" s="10" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:38" x14ac:dyDescent="0.25">
@@ -7462,16 +7462,16 @@
         <v>0.1.20-Gargantulus</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G22" s="10">
         <v>1</v>
@@ -7578,16 +7578,16 @@
         <v>{fire} {bullets} {punch} {scratch} {acid}</v>
       </c>
       <c r="AI22" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ22" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK22" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL22" s="10" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="23" spans="1:38" x14ac:dyDescent="0.25">
@@ -7599,16 +7599,16 @@
         <v>0.1.21-Akkorokamui</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F23" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G23" s="10">
         <v>1</v>
@@ -7715,16 +7715,16 @@
         <v>{fire} {bullets} {electricity} {scratch} {acid}</v>
       </c>
       <c r="AI23" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ23" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK23" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL23" s="10" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:38" x14ac:dyDescent="0.25">
@@ -7736,16 +7736,16 @@
         <v>0.1.22-Birgus Gigantus</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F24" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G24" s="10">
         <v>1</v>
@@ -7852,16 +7852,16 @@
         <v>{fire} {bullets} {electricity} {punch} {acid}</v>
       </c>
       <c r="AI24" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ24" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK24" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL24" s="10" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:38" x14ac:dyDescent="0.25">
@@ -7873,16 +7873,16 @@
         <v>0.1.23-Kaidoro</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F25" s="10" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G25" s="10">
         <v>1</v>
@@ -7989,16 +7989,16 @@
         <v>{fire} {bullets} {electricity} {punch} {scratch}</v>
       </c>
       <c r="AI25" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="AJ25" s="10" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AK25" s="10" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="AL25" s="10" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="26" spans="1:38" x14ac:dyDescent="0.25">
@@ -8010,16 +8010,16 @@
         <v>0.1.24-King Kaiju</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E26" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G26" s="10">
         <v>1</v>
@@ -8128,16 +8128,16 @@
         <v>{fire} {bullets} {electricity} {punch} {scratch} {acid}</v>
       </c>
       <c r="AI26" s="10" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AJ26" s="10" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="AK26" s="10" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="AL26" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:38" x14ac:dyDescent="0.25">
@@ -8149,16 +8149,16 @@
         <v>0.1.25-Lady Balkoth</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>53</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G27" s="10">
         <v>1</v>
@@ -8267,16 +8267,16 @@
         <v>{fire} {bullets} {electricity} {punch} {scratch} {acid}</v>
       </c>
       <c r="AI27" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="AJ27" s="10" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="AK27" s="10" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="AL27" s="10" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
   </sheetData>
@@ -8312,7 +8312,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -8360,13 +8360,13 @@
         <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8390,13 +8390,13 @@
         <v>16</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -8420,13 +8420,13 @@
         <v>17</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -8450,13 +8450,13 @@
         <v>18</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>19</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -8480,13 +8480,13 @@
         <v>20</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -8510,13 +8510,13 @@
         <v>22</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H7" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -8540,13 +8540,13 @@
         <v>32</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
@@ -8570,13 +8570,13 @@
         <v>33</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
@@ -8600,13 +8600,13 @@
         <v>34</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -8630,13 +8630,13 @@
         <v>35</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -8660,13 +8660,13 @@
         <v>36</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H12" s="3" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -8687,16 +8687,16 @@
         <v>41</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
@@ -8717,16 +8717,16 @@
         <v>41</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H14" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -8750,13 +8750,13 @@
         <v>42</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -8777,16 +8777,16 @@
         <v>41</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G16" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>15</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -8810,13 +8810,13 @@
         <v>43</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H17" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -8840,13 +8840,13 @@
         <v>44</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>21</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -8870,13 +8870,13 @@
         <v>45</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H19" s="3" t="s">
         <v>15</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -8910,7 +8910,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -8949,22 +8949,22 @@
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -8979,22 +8979,22 @@
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>31</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
@@ -9009,22 +9009,22 @@
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="H4" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -9039,22 +9039,22 @@
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -9069,22 +9069,22 @@
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>21</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
   </sheetData>
@@ -9122,7 +9122,7 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -9146,7 +9146,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>10</v>
@@ -9170,7 +9170,7 @@
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>13</v>
@@ -9179,14 +9179,14 @@
         <v>24</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
@@ -9204,7 +9204,7 @@
         <v>23</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>13</v>
@@ -9213,14 +9213,14 @@
         <v>25</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" s="3"/>
       <c r="J3" s="7" t="s">
         <v>27</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
@@ -9238,7 +9238,7 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>13</v>
@@ -9247,14 +9247,14 @@
         <v>26</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I4" s="3"/>
       <c r="J4" s="7" t="s">
         <v>19</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
@@ -9272,7 +9272,7 @@
         <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>13</v>
@@ -9281,14 +9281,14 @@
         <v>28</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="I5" s="3"/>
       <c r="J5" s="7" t="s">
         <v>21</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
@@ -9306,7 +9306,7 @@
         <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>31</v>
@@ -9315,14 +9315,14 @@
         <v>37</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="I6" s="3"/>
       <c r="J6" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
@@ -9340,7 +9340,7 @@
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>31</v>
@@ -9349,14 +9349,14 @@
         <v>38</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I7" s="3"/>
       <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
@@ -9374,7 +9374,7 @@
         <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>31</v>
@@ -9383,14 +9383,14 @@
         <v>39</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="7" t="s">
         <v>21</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
@@ -9408,7 +9408,7 @@
         <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>41</v>
@@ -9417,14 +9417,14 @@
         <v>46</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="I9" s="3"/>
       <c r="J9" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
@@ -9442,7 +9442,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>41</v>
@@ -9451,14 +9451,14 @@
         <v>47</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="7" t="s">
         <v>30</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
@@ -9476,7 +9476,7 @@
         <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="3" t="s">
         <v>41</v>
@@ -9485,14 +9485,14 @@
         <v>48</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I11" s="3"/>
       <c r="J11" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -9510,7 +9510,7 @@
         <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>41</v>
@@ -9519,14 +9519,14 @@
         <v>49</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="7" t="s">
         <v>30</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
@@ -9544,22 +9544,22 @@
         <v>23</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>41</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="J13" s="3" t="s">
         <v>15</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.25">
@@ -9577,7 +9577,7 @@
         <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>41</v>
@@ -9586,14 +9586,14 @@
         <v>50</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3" t="s">
         <v>30</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
@@ -9611,7 +9611,7 @@
         <v>23</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="13" t="s">
         <v>13</v>
@@ -9620,14 +9620,14 @@
         <v>29</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I15" s="8"/>
       <c r="J15" s="13" t="s">
         <v>30</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
@@ -9645,7 +9645,7 @@
         <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F16" s="13" t="s">
         <v>31</v>
@@ -9654,14 +9654,14 @@
         <v>40</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I16" s="8"/>
       <c r="J16" s="13" t="s">
         <v>30</v>
       </c>
       <c r="K16" s="13" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -9679,21 +9679,21 @@
         <v>23</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F17" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G17" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="J17" s="8"/>
       <c r="K17" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
@@ -9711,7 +9711,7 @@
         <v>23</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>51</v>
@@ -9721,11 +9721,11 @@
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="5" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="J18" s="8"/>
       <c r="K18" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
@@ -9743,21 +9743,21 @@
         <v>23</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="J19" s="8"/>
       <c r="K19" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -9775,21 +9775,21 @@
         <v>23</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F20" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="J20" s="8"/>
       <c r="K20" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -9807,21 +9807,21 @@
         <v>23</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F21" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H21" s="8"/>
       <c r="I21" s="5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="J21" s="8"/>
       <c r="K21" s="13" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -9857,7 +9857,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -9881,7 +9881,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>66</v>
@@ -9902,20 +9902,20 @@
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -9933,20 +9933,20 @@
         <v>23</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="5" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -9964,20 +9964,20 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -9995,20 +9995,20 @@
         <v>23</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="5" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -10026,20 +10026,20 @@
         <v>23</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="5" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -10057,20 +10057,20 @@
         <v>23</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -10088,20 +10088,20 @@
         <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -10119,20 +10119,20 @@
         <v>23</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -10150,20 +10150,20 @@
         <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -10181,20 +10181,20 @@
         <v>23</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="J11" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10212,20 +10212,20 @@
         <v>23</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="5" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="J12" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -10243,20 +10243,20 @@
         <v>23</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="5" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -10274,20 +10274,20 @@
         <v>23</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="5" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J14" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10305,20 +10305,20 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="J15" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -10336,20 +10336,20 @@
         <v>23</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J16" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -10367,20 +10367,20 @@
         <v>23</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -10398,20 +10398,20 @@
         <v>23</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -10429,20 +10429,20 @@
         <v>23</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -10460,20 +10460,20 @@
         <v>23</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="5" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -10491,20 +10491,20 @@
         <v>23</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -10545,7 +10545,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -10569,7 +10569,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>66</v>
@@ -10590,18 +10590,18 @@
         <v>23</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>288</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>289</v>
       </c>
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -10619,18 +10619,18 @@
         <v>23</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H3" s="8"/>
       <c r="I3" s="5"/>
       <c r="J3" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -10648,18 +10648,18 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="H4" s="8"/>
       <c r="I4" s="5"/>
       <c r="J4" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -10677,18 +10677,18 @@
         <v>23</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H5" s="8"/>
       <c r="I5" s="5"/>
       <c r="J5" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -10706,18 +10706,18 @@
         <v>23</v>
       </c>
       <c r="E6" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="H6" s="8"/>
       <c r="I6" s="5"/>
       <c r="J6" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -10735,18 +10735,18 @@
         <v>23</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H7" s="8"/>
       <c r="I7" s="5"/>
       <c r="J7" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -10764,18 +10764,18 @@
         <v>23</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H8" s="8"/>
       <c r="I8" s="5"/>
       <c r="J8" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -10793,18 +10793,18 @@
         <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>293</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>294</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="G9" s="5" t="s">
-        <v>295</v>
       </c>
       <c r="H9" s="8"/>
       <c r="I9" s="5"/>
       <c r="J9" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -10822,18 +10822,18 @@
         <v>23</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H10" s="8"/>
       <c r="I10" s="5"/>
       <c r="J10" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -10851,18 +10851,18 @@
         <v>23</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="H11" s="8"/>
       <c r="I11" s="5"/>
       <c r="J11" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -10880,18 +10880,18 @@
         <v>23</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H12" s="8"/>
       <c r="I12" s="5"/>
       <c r="J12" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -10909,18 +10909,18 @@
         <v>23</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="H13" s="8"/>
       <c r="I13" s="5"/>
       <c r="J13" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -10938,18 +10938,18 @@
         <v>23</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H14" s="8"/>
       <c r="I14" s="5"/>
       <c r="J14" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -10967,18 +10967,18 @@
         <v>23</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H15" s="8"/>
       <c r="I15" s="5"/>
       <c r="J15" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -10996,18 +10996,18 @@
         <v>23</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G16" s="14" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="H16" s="14"/>
       <c r="I16" s="14"/>
       <c r="J16" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -11025,18 +11025,18 @@
         <v>23</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F17" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="H17" s="8"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -11054,18 +11054,18 @@
         <v>23</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F18" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="H18" s="8"/>
       <c r="I18" s="8"/>
       <c r="J18" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -11083,18 +11083,18 @@
         <v>23</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F19" s="8" t="s">
         <v>51</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H19" s="8"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -11112,18 +11112,18 @@
         <v>23</v>
       </c>
       <c r="E20" s="12" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F20" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="H20" s="8"/>
       <c r="I20" s="5"/>
       <c r="J20" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -11141,18 +11141,18 @@
         <v>23</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="F21" s="5" t="s">
         <v>51</v>
       </c>
       <c r="G21" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H21" s="15"/>
       <c r="I21" s="15"/>
       <c r="J21" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -11168,7 +11168,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EF6E018-AD1D-4BFD-9424-9832D8579396}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -11186,7 +11186,7 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
@@ -11198,10 +11198,10 @@
         <v>2</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>311</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>312</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>313</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
@@ -11215,24 +11215,24 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="str">
-        <f>CONCATENATE("3.2.",A2,"-",G2)</f>
+        <f t="shared" ref="B2:B19" si="0">CONCATENATE("3.2.",A2,"-",G2)</f>
         <v>3.2.0-</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -11240,24 +11240,24 @@
         <v>1</v>
       </c>
       <c r="B3" s="8" t="str">
-        <f>CONCATENATE("3.2.",A3,"-",G3)</f>
+        <f t="shared" si="0"/>
         <v>3.2.1-</v>
       </c>
       <c r="C3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="G3" s="5"/>
       <c r="H3" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -11265,24 +11265,24 @@
         <v>2</v>
       </c>
       <c r="B4" s="8" t="str">
-        <f>CONCATENATE("3.2.",A4,"-",G4)</f>
+        <f t="shared" si="0"/>
         <v>3.2.2-</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E4" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="F4" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G4" s="5"/>
       <c r="H4" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -11290,24 +11290,24 @@
         <v>3</v>
       </c>
       <c r="B5" s="8" t="str">
-        <f>CONCATENATE("3.2.",A5,"-",G5)</f>
+        <f t="shared" si="0"/>
         <v>3.2.3-</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="F5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G5" s="5"/>
       <c r="H5" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -11315,24 +11315,24 @@
         <v>4</v>
       </c>
       <c r="B6" s="8" t="str">
-        <f>CONCATENATE("3.2.",A6,"-",G6)</f>
+        <f t="shared" si="0"/>
         <v>3.2.4-</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E6" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F6" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="G6" s="5"/>
       <c r="H6" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -11340,24 +11340,24 @@
         <v>5</v>
       </c>
       <c r="B7" s="8" t="str">
-        <f>CONCATENATE("3.2.",A7,"-",G7)</f>
+        <f t="shared" si="0"/>
         <v>3.2.5-</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>320</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>321</v>
       </c>
       <c r="G7" s="5"/>
       <c r="H7" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -11365,24 +11365,24 @@
         <v>6</v>
       </c>
       <c r="B8" s="8" t="str">
-        <f>CONCATENATE("3.2.",A8,"-",G8)</f>
+        <f t="shared" si="0"/>
         <v>3.2.6-</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -11390,24 +11390,24 @@
         <v>7</v>
       </c>
       <c r="B9" s="8" t="str">
-        <f>CONCATENATE("3.2.",A9,"-",G9)</f>
+        <f t="shared" si="0"/>
         <v>3.2.7-</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G9" s="5"/>
       <c r="H9" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -11415,24 +11415,24 @@
         <v>8</v>
       </c>
       <c r="B10" s="8" t="str">
-        <f>CONCATENATE("3.2.",A10,"-",G10)</f>
+        <f t="shared" si="0"/>
         <v>3.2.8-</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E10" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="F10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -11440,24 +11440,24 @@
         <v>9</v>
       </c>
       <c r="B11" s="8" t="str">
-        <f>CONCATENATE("3.2.",A11,"-",G11)</f>
+        <f t="shared" si="0"/>
         <v>3.2.9-</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="F11" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -11465,24 +11465,24 @@
         <v>10</v>
       </c>
       <c r="B12" s="8" t="str">
-        <f>CONCATENATE("3.2.",A12,"-",G12)</f>
+        <f t="shared" si="0"/>
         <v>3.2.10-</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E12" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="F12" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="G12" s="5"/>
       <c r="H12" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -11490,24 +11490,24 @@
         <v>11</v>
       </c>
       <c r="B13" s="8" t="str">
-        <f>CONCATENATE("3.2.",A13,"-",G13)</f>
+        <f t="shared" si="0"/>
         <v>3.2.11-</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="F13" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="G13" s="5"/>
       <c r="H13" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -11515,24 +11515,24 @@
         <v>12</v>
       </c>
       <c r="B14" s="8" t="str">
-        <f>CONCATENATE("3.2.",A14,"-",G14)</f>
+        <f t="shared" si="0"/>
         <v>3.2.12-</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="G14" s="5"/>
       <c r="H14" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -11540,24 +11540,24 @@
         <v>13</v>
       </c>
       <c r="B15" s="8" t="str">
-        <f>CONCATENATE("3.2.",A15,"-",G15)</f>
+        <f t="shared" si="0"/>
         <v>3.2.13-</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="F15" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="G15" s="5"/>
       <c r="H15" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -11565,24 +11565,24 @@
         <v>14</v>
       </c>
       <c r="B16" s="8" t="str">
-        <f>CONCATENATE("3.2.",A16,"-",G16)</f>
+        <f t="shared" si="0"/>
         <v>3.2.14-</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E16" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="F16" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G16" s="14"/>
       <c r="H16" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -11590,24 +11590,24 @@
         <v>15</v>
       </c>
       <c r="B17" s="8" t="str">
-        <f>CONCATENATE("3.2.",A17,"-",G17)</f>
+        <f t="shared" si="0"/>
         <v>3.2.15-</v>
       </c>
       <c r="C17" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E17" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="F17" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="G17" s="5"/>
       <c r="H17" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -11615,24 +11615,24 @@
         <v>16</v>
       </c>
       <c r="B18" s="8" t="str">
-        <f>CONCATENATE("3.2.",A18,"-",G18)</f>
+        <f t="shared" si="0"/>
         <v>3.2.16-</v>
       </c>
       <c r="C18" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G18" s="5"/>
       <c r="H18" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -11640,24 +11640,24 @@
         <v>17</v>
       </c>
       <c r="B19" s="8" t="str">
-        <f>CONCATENATE("3.2.",A19,"-",G19)</f>
+        <f t="shared" si="0"/>
         <v>3.2.17-</v>
       </c>
       <c r="C19" s="5" t="s">
         <v>11</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E19" s="16" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="G19" s="5"/>
       <c r="H19" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
   </sheetData>

</xml_diff>